<commit_message>
Doc from firts meeting and begining of third sprint
</commit_message>
<xml_diff>
--- a/docs/MapaEntregables.xlsx
+++ b/docs/MapaEntregables.xlsx
@@ -1,13 +1,8 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr updateLinks="always" codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian\Documents\UBA\2do Cuat 2013\TallerDesarrollo2\docs\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
@@ -48,7 +43,7 @@
     <definedName name="VacationStartDates" localSheetId="0">'[1]w-plan'!#REF!</definedName>
     <definedName name="VacationStartDates">'[1]w-plan'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="124519"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -58,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
   <si>
     <t>Code/Implementation</t>
   </si>
@@ -163,18 +158,66 @@
   </si>
   <si>
     <t>Feriado: 14 Oct</t>
+  </si>
+  <si>
+    <t>Ver funciones</t>
+  </si>
+  <si>
+    <t>Admin. Crear Funcion</t>
+  </si>
+  <si>
+    <t>Admin. Listar Funcion</t>
+  </si>
+  <si>
+    <t>Admin. Editar Funcion</t>
+  </si>
+  <si>
+    <t>Admin. Disponibilidad Funcion</t>
+  </si>
+  <si>
+    <t>Admin. Borrar Funcion</t>
+  </si>
+  <si>
+    <t>Admin. Crear Sala</t>
+  </si>
+  <si>
+    <t>Admin. Listar Sala</t>
+  </si>
+  <si>
+    <t>Admin. Editar Sala</t>
+  </si>
+  <si>
+    <t>Admin. Borrar Sala</t>
+  </si>
+  <si>
+    <t>Usuarios con permisos (Read-only)</t>
+  </si>
+  <si>
+    <t>Estilos de salas</t>
+  </si>
+  <si>
+    <t>Compartir película en Tw y Fb</t>
+  </si>
+  <si>
+    <t>Ver Complejos</t>
+  </si>
+  <si>
+    <t>Ver Informacion de Complejo</t>
+  </si>
+  <si>
+    <t>Ver Cartelera de Complejo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;Iteration&quot;\ 0"/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -261,22 +304,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="16">
+  <borders count="14">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1"/>
-      </left>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -286,24 +318,6 @@
       <top style="thin">
         <color theme="1"/>
       </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color theme="1" tint="0.34998626667073579"/>
-      </left>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -366,29 +380,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
-      <top style="thin">
-        <color auto="1"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
       <right/>
-      <top/>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color theme="0" tint="-0.249977111117893"/>
-      </right>
       <top/>
       <bottom style="thin">
         <color indexed="64"/>
@@ -407,8 +399,30 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color theme="1"/>
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
       </left>
       <right/>
       <top/>
@@ -419,12 +433,19 @@
     </border>
     <border>
       <left style="thin">
-        <color auto="1"/>
+        <color indexed="64"/>
       </left>
       <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
       <bottom/>
       <diagonal/>
     </border>
@@ -433,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="40">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -442,16 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -467,153 +479,130 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="14" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="165" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Comma 2" xfId="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor theme="0" tint="-0.14996795556505021"/>
-        </patternFill>
-      </fill>
-      <border>
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <vertical/>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="3" tint="0.39994506668294322"/>
-      </font>
-    </dxf>
+  <dxfs count="2">
     <dxf>
       <fill>
         <patternFill>
@@ -655,13 +644,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>35718</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>97633</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>250031</xdr:colOff>
-      <xdr:row>18</xdr:row>
+      <xdr:row>29</xdr:row>
       <xdr:rowOff>330199</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -697,13 +686,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>264</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>61914</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>227276</xdr:colOff>
-      <xdr:row>19</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>307976</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -737,13 +726,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>228571</xdr:colOff>
-      <xdr:row>22</xdr:row>
+      <xdr:row>33</xdr:row>
       <xdr:rowOff>190471</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -775,13 +764,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>20637</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>230161</xdr:colOff>
-      <xdr:row>24</xdr:row>
+      <xdr:row>35</xdr:row>
       <xdr:rowOff>190474</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -813,13 +802,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>235716</xdr:colOff>
-      <xdr:row>20</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>266701</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -851,13 +840,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>235714</xdr:colOff>
-      <xdr:row>21</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>190476</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -889,13 +878,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>66675</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>265083</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>34</xdr:row>
       <xdr:rowOff>190471</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -927,13 +916,13 @@
     <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>27826</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>64559</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>3</xdr:col>
       <xdr:colOff>242138</xdr:colOff>
-      <xdr:row>17</xdr:row>
+      <xdr:row>28</xdr:row>
       <xdr:rowOff>291568</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1191,16 +1180,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>36634</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>73269</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>250946</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>300278</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>43961</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>87923</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>258273</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>314932</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1217,7 +1206,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="4769826" y="1597269"/>
+          <a:off x="5055576" y="1611923"/>
           <a:ext cx="214312" cy="227009"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1229,15 +1218,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>21981</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>58615</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>236293</xdr:colOff>
-      <xdr:row>8</xdr:row>
+      <xdr:row>11</xdr:row>
       <xdr:rowOff>285624</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1267,15 +1256,15 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>27842</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>93784</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>242154</xdr:colOff>
-      <xdr:row>9</xdr:row>
+      <xdr:row>12</xdr:row>
       <xdr:rowOff>320793</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
@@ -1305,16 +1294,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>21980</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:row>13</xdr:row>
       <xdr:rowOff>7326</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>13</xdr:col>
+      <xdr:col>8</xdr:col>
       <xdr:colOff>236292</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>43835</xdr:rowOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>234335</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1343,16 +1332,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>36634</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>124558</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>13</xdr:col>
-      <xdr:colOff>250946</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>351567</xdr:rowOff>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>58616</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>243619</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>285625</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1369,7 +1358,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5048249" y="2894135"/>
+          <a:off x="5040922" y="2828193"/>
           <a:ext cx="214312" cy="227009"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1599,8 +1588,8 @@
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>302236</xdr:colOff>
-      <xdr:row>11</xdr:row>
-      <xdr:rowOff>49393</xdr:rowOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>239893</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -1747,20 +1736,58 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>51288</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>80596</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>265600</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>307605</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="34" name="Picture 33" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="3377711" y="2278673"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>43961</xdr:colOff>
+      <xdr:colOff>29307</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>95250</xdr:rowOff>
+      <xdr:rowOff>124558</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>13</xdr:col>
-      <xdr:colOff>258273</xdr:colOff>
+      <xdr:colOff>243619</xdr:colOff>
       <xdr:row>6</xdr:row>
-      <xdr:rowOff>322259</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="34" name="Picture 33" descr="source_code_32.png"/>
+      <xdr:rowOff>351567</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="58" name="Picture 34" descr="source_code_32.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1773,7 +1800,615 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="5055576" y="1238250"/>
+          <a:off x="5040922" y="1267558"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>29307</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>80596</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>243619</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>307605</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="59" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5040922" y="1604596"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>35169</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>35169</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>249481</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>262178</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="60" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5046784" y="1940169"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>41030</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>92319</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>255342</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>319328</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="61" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5052645" y="2290396"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>61544</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>46894</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>275856</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>273903</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="62" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5073159" y="2625971"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>74731</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>60085</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>289043</xdr:colOff>
+      <xdr:row>11</xdr:row>
+      <xdr:rowOff>287094</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="63" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5086346" y="3027489"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>65937</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>80603</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>280249</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>307612</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="64" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5077552" y="3407026"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>79124</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>35178</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>293436</xdr:colOff>
+      <xdr:row>13</xdr:row>
+      <xdr:rowOff>262187</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="65" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5090739" y="3749928"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>77657</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>99657</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>291969</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>326666</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="66" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5089272" y="4122138"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>105498</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>98195</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>319810</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>325204</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="67" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5117113" y="4530983"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>118685</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>96732</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>332997</xdr:colOff>
+      <xdr:row>16</xdr:row>
+      <xdr:rowOff>323741</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="68" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5130300" y="4939828"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>124545</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>95269</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>1818</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>322278</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="69" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5136160" y="5348673"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>115751</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>101133</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>330063</xdr:colOff>
+      <xdr:row>18</xdr:row>
+      <xdr:rowOff>328142</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="70" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5127366" y="5764845"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>121611</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>99671</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>335923</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>326680</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="71" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5133226" y="6173690"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>127471</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>98208</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>4744</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>325217</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="72" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5139086" y="6582535"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>133331</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>89418</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>10604</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>316427</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="73" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5144946" y="6984053"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>139191</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>87956</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>16464</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>314965</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="74" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="5150806" y="7392898"/>
           <a:ext cx="214312" cy="227009"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1787,7 +2422,7 @@
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="w-plan"/>
@@ -1818,7 +2453,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1860,7 +2495,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1892,10 +2527,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1927,7 +2561,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2103,29 +2736,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A4:AB26"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A4:AB37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="K6" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="N13" sqref="N13:R13"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C22" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4:R24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
     <col min="3" max="3" width="7.42578125" style="1" customWidth="1"/>
-    <col min="4" max="22" width="5" style="1" customWidth="1"/>
+    <col min="4" max="17" width="5" style="1" customWidth="1"/>
+    <col min="18" max="18" width="14.85546875" style="1" customWidth="1"/>
+    <col min="19" max="22" width="5" style="1" customWidth="1"/>
     <col min="23" max="23" width="6.140625" style="1" customWidth="1"/>
     <col min="24" max="54" width="5" style="1" customWidth="1"/>
     <col min="55" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="23" t="s">
+    <row r="4" spans="1:28">
+      <c r="A4" s="17" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="23"/>
+      <c r="B4" s="17"/>
       <c r="D4" s="33" t="s">
         <v>14</v>
       </c>
@@ -2133,13 +2768,13 @@
       <c r="F4" s="34"/>
       <c r="G4" s="34"/>
       <c r="H4" s="35"/>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="18" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="34"/>
-      <c r="K4" s="34"/>
-      <c r="L4" s="34"/>
-      <c r="M4" s="35"/>
+      <c r="J4" s="18"/>
+      <c r="K4" s="18"/>
+      <c r="L4" s="18"/>
+      <c r="M4" s="19"/>
       <c r="N4" s="33" t="s">
         <v>16</v>
       </c>
@@ -2147,7 +2782,7 @@
       <c r="P4" s="34"/>
       <c r="Q4" s="34"/>
       <c r="R4" s="35"/>
-      <c r="S4" s="36" t="s">
+      <c r="S4" s="33" t="s">
         <v>17</v>
       </c>
       <c r="T4" s="34"/>
@@ -2162,485 +2797,862 @@
       <c r="AA4" s="34"/>
       <c r="AB4" s="35"/>
     </row>
-    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D5" s="37" t="s">
+    <row r="5" spans="1:28">
+      <c r="D5" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="38"/>
-      <c r="F5" s="38"/>
-      <c r="G5" s="38"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="37" t="s">
+      <c r="E5" s="20"/>
+      <c r="F5" s="20"/>
+      <c r="G5" s="20"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="41" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="38"/>
-      <c r="K5" s="38"/>
-      <c r="L5" s="38"/>
-      <c r="M5" s="39"/>
-      <c r="N5" s="37" t="s">
+      <c r="J5" s="42"/>
+      <c r="K5" s="42"/>
+      <c r="L5" s="42"/>
+      <c r="M5" s="43"/>
+      <c r="N5" s="36" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="38"/>
-      <c r="P5" s="38"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="39"/>
-      <c r="S5" s="37" t="s">
+      <c r="O5" s="20"/>
+      <c r="P5" s="20"/>
+      <c r="Q5" s="20"/>
+      <c r="R5" s="21"/>
+      <c r="S5" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="38"/>
-      <c r="U5" s="38"/>
-      <c r="V5" s="38"/>
-      <c r="W5" s="39"/>
-      <c r="X5" s="37" t="s">
+      <c r="T5" s="20"/>
+      <c r="U5" s="20"/>
+      <c r="V5" s="20"/>
+      <c r="W5" s="21"/>
+      <c r="X5" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="Y5" s="38"/>
-      <c r="Z5" s="38"/>
-      <c r="AA5" s="38"/>
-      <c r="AB5" s="39"/>
+      <c r="Y5" s="20"/>
+      <c r="Z5" s="20"/>
+      <c r="AA5" s="20"/>
+      <c r="AB5" s="21"/>
     </row>
-    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D6" s="5"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
-      <c r="K6" s="6"/>
-      <c r="L6" s="6"/>
-      <c r="M6" s="7"/>
-      <c r="N6" s="6"/>
-      <c r="O6" s="6"/>
-      <c r="P6" s="6"/>
-      <c r="Q6" s="6"/>
-      <c r="R6" s="7"/>
-      <c r="S6" s="6"/>
-      <c r="T6" s="6"/>
-      <c r="U6" s="6"/>
-      <c r="V6" s="6"/>
-      <c r="W6" s="7"/>
-      <c r="X6" s="6"/>
-      <c r="Y6" s="6"/>
-      <c r="Z6" s="6"/>
-      <c r="AA6" s="6"/>
-      <c r="AB6" s="7"/>
+    <row r="6" spans="1:28">
+      <c r="D6" s="4"/>
+      <c r="E6" s="27"/>
+      <c r="F6" s="27"/>
+      <c r="G6" s="27"/>
+      <c r="H6" s="28"/>
+      <c r="I6" s="44"/>
+      <c r="J6" s="27"/>
+      <c r="K6" s="27"/>
+      <c r="L6" s="27"/>
+      <c r="M6" s="28"/>
+      <c r="N6" s="44"/>
+      <c r="O6" s="27"/>
+      <c r="P6" s="27"/>
+      <c r="Q6" s="27"/>
+      <c r="R6" s="28"/>
+      <c r="S6" s="44"/>
+      <c r="T6" s="27"/>
+      <c r="U6" s="27"/>
+      <c r="V6" s="27"/>
+      <c r="W6" s="28"/>
+      <c r="X6" s="44"/>
+      <c r="Y6" s="27"/>
+      <c r="Z6" s="27"/>
+      <c r="AA6" s="27"/>
+      <c r="AB6" s="28"/>
     </row>
-    <row r="7" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D7" s="4"/>
-      <c r="E7" s="31" t="s">
+    <row r="7" spans="1:28" ht="30" customHeight="1">
+      <c r="D7" s="37"/>
+      <c r="E7" s="22" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="31"/>
-      <c r="G7" s="31"/>
-      <c r="H7" s="32"/>
-      <c r="I7" s="3"/>
-      <c r="J7" s="31" t="s">
+      <c r="F7" s="22"/>
+      <c r="G7" s="22"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="37"/>
+      <c r="J7" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="31"/>
-      <c r="L7" s="31"/>
-      <c r="M7" s="32"/>
-      <c r="N7" s="3"/>
-      <c r="O7" s="31" t="s">
+      <c r="K7" s="22"/>
+      <c r="L7" s="22"/>
+      <c r="M7" s="38"/>
+      <c r="N7" s="37"/>
+      <c r="O7" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="P7" s="22"/>
+      <c r="Q7" s="22"/>
+      <c r="R7" s="38"/>
+      <c r="S7" s="37"/>
+      <c r="T7" s="22"/>
+      <c r="U7" s="22"/>
+      <c r="V7" s="22"/>
+      <c r="W7" s="38"/>
+      <c r="X7" s="37"/>
+      <c r="Y7" s="22"/>
+      <c r="Z7" s="22"/>
+      <c r="AA7" s="22"/>
+      <c r="AB7" s="38"/>
+    </row>
+    <row r="8" spans="1:28" ht="30" customHeight="1">
+      <c r="D8" s="37"/>
+      <c r="E8" s="22" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="22"/>
+      <c r="G8" s="22"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="37"/>
+      <c r="J8" s="22" t="s">
+        <v>25</v>
+      </c>
+      <c r="K8" s="22"/>
+      <c r="L8" s="22"/>
+      <c r="M8" s="38"/>
+      <c r="N8" s="45"/>
+      <c r="O8" s="22" t="s">
+        <v>36</v>
+      </c>
+      <c r="P8" s="22"/>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="38"/>
+      <c r="S8" s="37"/>
+      <c r="T8" s="22"/>
+      <c r="U8" s="22"/>
+      <c r="V8" s="22"/>
+      <c r="W8" s="38"/>
+      <c r="X8" s="37"/>
+      <c r="Y8" s="22"/>
+      <c r="Z8" s="22"/>
+      <c r="AA8" s="22"/>
+      <c r="AB8" s="38"/>
+    </row>
+    <row r="9" spans="1:28" ht="23.25" customHeight="1">
+      <c r="D9" s="37"/>
+      <c r="E9" s="22" t="s">
+        <v>13</v>
+      </c>
+      <c r="F9" s="22"/>
+      <c r="G9" s="22"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="22" t="s">
+        <v>26</v>
+      </c>
+      <c r="K9" s="22"/>
+      <c r="L9" s="22"/>
+      <c r="M9" s="38"/>
+      <c r="N9" s="45"/>
+      <c r="O9" s="22" t="s">
+        <v>37</v>
+      </c>
+      <c r="P9" s="22"/>
+      <c r="Q9" s="22"/>
+      <c r="R9" s="38"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="22"/>
+      <c r="U9" s="22"/>
+      <c r="V9" s="22"/>
+      <c r="W9" s="38"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="22"/>
+      <c r="Z9" s="22"/>
+      <c r="AA9" s="22"/>
+      <c r="AB9" s="38"/>
+    </row>
+    <row r="10" spans="1:28" ht="30" customHeight="1">
+      <c r="D10" s="37"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="13"/>
+      <c r="H10" s="39"/>
+      <c r="I10" s="37"/>
+      <c r="J10" s="22" t="s">
         <v>28</v>
       </c>
-      <c r="P7" s="31"/>
-      <c r="Q7" s="31"/>
-      <c r="R7" s="32"/>
-      <c r="S7" s="3"/>
-      <c r="T7" s="31"/>
-      <c r="U7" s="31"/>
-      <c r="V7" s="31"/>
-      <c r="W7" s="32"/>
-      <c r="X7" s="3"/>
-      <c r="Y7" s="31"/>
-      <c r="Z7" s="31"/>
-      <c r="AA7" s="31"/>
-      <c r="AB7" s="32"/>
+      <c r="K10" s="22"/>
+      <c r="L10" s="22"/>
+      <c r="M10" s="38"/>
+      <c r="N10" s="45"/>
+      <c r="O10" s="22" t="s">
+        <v>38</v>
+      </c>
+      <c r="P10" s="22"/>
+      <c r="Q10" s="22"/>
+      <c r="R10" s="38"/>
+      <c r="S10" s="37"/>
+      <c r="T10" s="22"/>
+      <c r="U10" s="22"/>
+      <c r="V10" s="22"/>
+      <c r="W10" s="38"/>
+      <c r="X10" s="37"/>
+      <c r="Y10" s="22"/>
+      <c r="Z10" s="22"/>
+      <c r="AA10" s="22"/>
+      <c r="AB10" s="38"/>
     </row>
-    <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D8" s="4"/>
-      <c r="E8" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="F8" s="18"/>
-      <c r="G8" s="18"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="18" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="18"/>
-      <c r="L8" s="18"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="3"/>
-      <c r="O8" s="18" t="s">
+    <row r="11" spans="1:28" ht="30.75" customHeight="1">
+      <c r="D11" s="37"/>
+      <c r="E11" s="13"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="13"/>
+      <c r="H11" s="39"/>
+      <c r="I11" s="37"/>
+      <c r="J11" s="22" t="s">
         <v>29</v>
       </c>
-      <c r="P8" s="18"/>
-      <c r="Q8" s="18"/>
-      <c r="R8" s="19"/>
-      <c r="S8" s="3"/>
-      <c r="T8" s="18"/>
-      <c r="U8" s="18"/>
-      <c r="V8" s="18"/>
-      <c r="W8" s="19"/>
-      <c r="X8" s="3"/>
-      <c r="Y8" s="18"/>
-      <c r="Z8" s="18"/>
-      <c r="AA8" s="18"/>
-      <c r="AB8" s="19"/>
+      <c r="K11" s="22"/>
+      <c r="L11" s="22"/>
+      <c r="M11" s="38"/>
+      <c r="N11" s="45"/>
+      <c r="O11" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="P11" s="22"/>
+      <c r="Q11" s="22"/>
+      <c r="R11" s="38"/>
+      <c r="S11" s="37"/>
+      <c r="T11" s="13"/>
+      <c r="U11" s="13"/>
+      <c r="V11" s="13"/>
+      <c r="W11" s="39"/>
+      <c r="X11" s="37"/>
+      <c r="Y11" s="22"/>
+      <c r="Z11" s="22"/>
+      <c r="AA11" s="22"/>
+      <c r="AB11" s="38"/>
     </row>
-    <row r="9" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D9" s="4"/>
-      <c r="E9" s="18" t="s">
-        <v>13</v>
-      </c>
-      <c r="F9" s="18"/>
-      <c r="G9" s="18"/>
-      <c r="H9" s="19"/>
-      <c r="I9" s="3"/>
-      <c r="J9" s="18" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="18"/>
-      <c r="L9" s="18"/>
-      <c r="M9" s="19"/>
-      <c r="N9" s="3"/>
-      <c r="O9" s="18" t="s">
+    <row r="12" spans="1:28" ht="28.5" customHeight="1">
+      <c r="D12" s="37"/>
+      <c r="E12" s="13"/>
+      <c r="F12" s="13"/>
+      <c r="G12" s="13"/>
+      <c r="H12" s="39"/>
+      <c r="I12" s="37"/>
+      <c r="J12" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="P9" s="18"/>
-      <c r="Q9" s="18"/>
-      <c r="R9" s="19"/>
-      <c r="S9" s="3"/>
-      <c r="T9" s="18"/>
-      <c r="U9" s="18"/>
-      <c r="V9" s="18"/>
-      <c r="W9" s="19"/>
-      <c r="X9" s="3"/>
-      <c r="Y9" s="18"/>
-      <c r="Z9" s="18"/>
-      <c r="AA9" s="18"/>
-      <c r="AB9" s="19"/>
+      <c r="K12" s="22"/>
+      <c r="L12" s="22"/>
+      <c r="M12" s="38"/>
+      <c r="N12" s="45"/>
+      <c r="O12" s="22" t="s">
+        <v>40</v>
+      </c>
+      <c r="P12" s="22"/>
+      <c r="Q12" s="22"/>
+      <c r="R12" s="38"/>
+      <c r="S12" s="37"/>
+      <c r="T12" s="13"/>
+      <c r="U12" s="13"/>
+      <c r="V12" s="13"/>
+      <c r="W12" s="39"/>
+      <c r="X12" s="37"/>
+      <c r="Y12" s="13"/>
+      <c r="Z12" s="13"/>
+      <c r="AA12" s="13"/>
+      <c r="AB12" s="39"/>
     </row>
-    <row r="10" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="4"/>
-      <c r="E10" s="15"/>
-      <c r="F10" s="15"/>
-      <c r="G10" s="15"/>
-      <c r="H10" s="16"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="18"/>
-      <c r="K10" s="18"/>
-      <c r="L10" s="18"/>
-      <c r="M10" s="19"/>
-      <c r="N10" s="3"/>
-      <c r="O10" s="18" t="s">
+    <row r="13" spans="1:28" ht="30.75" customHeight="1">
+      <c r="D13" s="37"/>
+      <c r="E13" s="13"/>
+      <c r="F13" s="13"/>
+      <c r="G13" s="13"/>
+      <c r="H13" s="39"/>
+      <c r="I13" s="37"/>
+      <c r="J13" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="P10" s="18"/>
-      <c r="Q10" s="18"/>
-      <c r="R10" s="19"/>
-      <c r="S10" s="3"/>
-      <c r="T10" s="18"/>
-      <c r="U10" s="18"/>
-      <c r="V10" s="18"/>
-      <c r="W10" s="19"/>
-      <c r="X10" s="3"/>
-      <c r="Y10" s="18"/>
-      <c r="Z10" s="18"/>
-      <c r="AA10" s="18"/>
-      <c r="AB10" s="19"/>
+      <c r="K13" s="22"/>
+      <c r="L13" s="22"/>
+      <c r="M13" s="38"/>
+      <c r="N13" s="37"/>
+      <c r="O13" s="22" t="s">
+        <v>41</v>
+      </c>
+      <c r="P13" s="22"/>
+      <c r="Q13" s="22"/>
+      <c r="R13" s="38"/>
+      <c r="S13" s="37"/>
+      <c r="T13" s="13"/>
+      <c r="U13" s="13"/>
+      <c r="V13" s="13"/>
+      <c r="W13" s="39"/>
+      <c r="X13" s="37"/>
+      <c r="Y13" s="13"/>
+      <c r="Z13" s="13"/>
+      <c r="AA13" s="13"/>
+      <c r="AB13" s="39"/>
     </row>
-    <row r="11" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D11" s="4"/>
-      <c r="E11" s="15"/>
-      <c r="F11" s="15"/>
-      <c r="G11" s="15"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="3"/>
-      <c r="J11" s="15"/>
-      <c r="K11" s="15"/>
-      <c r="L11" s="15"/>
-      <c r="M11" s="16"/>
-      <c r="N11" s="3"/>
-      <c r="O11" s="18" t="s">
-        <v>32</v>
-      </c>
-      <c r="P11" s="18"/>
-      <c r="Q11" s="18"/>
-      <c r="R11" s="19"/>
-      <c r="S11" s="3"/>
-      <c r="T11" s="15"/>
-      <c r="U11" s="15"/>
-      <c r="V11" s="15"/>
-      <c r="W11" s="16"/>
-      <c r="X11" s="3"/>
-      <c r="Y11" s="18"/>
-      <c r="Z11" s="18"/>
-      <c r="AA11" s="18"/>
-      <c r="AB11" s="19"/>
-    </row>
-    <row r="12" spans="1:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D12" s="4"/>
-      <c r="E12" s="25"/>
-      <c r="F12" s="25"/>
-      <c r="G12" s="25"/>
-      <c r="H12" s="26"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="25"/>
-      <c r="K12" s="25"/>
-      <c r="L12" s="25"/>
-      <c r="M12" s="26"/>
-      <c r="N12" s="3"/>
-      <c r="O12" s="25" t="s">
-        <v>33</v>
-      </c>
-      <c r="P12" s="25"/>
-      <c r="Q12" s="25"/>
-      <c r="R12" s="26"/>
-      <c r="S12" s="3"/>
-      <c r="T12" s="27"/>
-      <c r="U12" s="27"/>
-      <c r="V12" s="27"/>
-      <c r="W12" s="28"/>
-      <c r="X12" s="3"/>
-      <c r="Y12" s="29"/>
-      <c r="Z12" s="29"/>
-      <c r="AA12" s="29"/>
-      <c r="AB12" s="30"/>
-    </row>
-    <row r="13" spans="1:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="B13" s="24"/>
-      <c r="D13" s="20" t="s">
-        <v>21</v>
-      </c>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="22"/>
-      <c r="I13" s="20"/>
-      <c r="J13" s="21"/>
-      <c r="K13" s="21"/>
-      <c r="L13" s="21"/>
-      <c r="M13" s="22"/>
-      <c r="N13" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="O13" s="21"/>
-      <c r="P13" s="21"/>
-      <c r="Q13" s="21"/>
-      <c r="R13" s="22"/>
-      <c r="S13" s="20"/>
-      <c r="T13" s="21"/>
-      <c r="U13" s="21"/>
-      <c r="V13" s="21"/>
-      <c r="W13" s="22"/>
-      <c r="X13" s="20"/>
-      <c r="Y13" s="21"/>
-      <c r="Z13" s="21"/>
-      <c r="AA13" s="21"/>
-      <c r="AB13" s="22"/>
-    </row>
-    <row r="14" spans="1:28" s="10" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
-      <c r="D14" s="13"/>
+    <row r="14" spans="1:28" ht="24" customHeight="1">
+      <c r="D14" s="37"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="13"/>
-      <c r="I14" s="14"/>
-      <c r="J14" s="14"/>
-      <c r="K14" s="14"/>
-      <c r="L14" s="14"/>
-      <c r="M14" s="14"/>
-      <c r="N14" s="14"/>
-      <c r="O14" s="14"/>
-      <c r="P14" s="14"/>
-      <c r="Q14" s="14"/>
-      <c r="R14" s="14"/>
-      <c r="S14" s="14"/>
-      <c r="T14" s="14"/>
-      <c r="U14" s="14"/>
-      <c r="V14" s="14"/>
-      <c r="W14" s="14"/>
+      <c r="H14" s="39"/>
+      <c r="I14" s="37"/>
+      <c r="J14" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="K14" s="22"/>
+      <c r="L14" s="22"/>
+      <c r="M14" s="38"/>
+      <c r="N14" s="37"/>
+      <c r="O14" s="22" t="s">
+        <v>42</v>
+      </c>
+      <c r="P14" s="22"/>
+      <c r="Q14" s="22"/>
+      <c r="R14" s="38"/>
+      <c r="S14" s="37"/>
+      <c r="T14" s="13"/>
+      <c r="U14" s="13"/>
+      <c r="V14" s="13"/>
+      <c r="W14" s="39"/>
+      <c r="X14" s="37"/>
+      <c r="Y14" s="13"/>
+      <c r="Z14" s="13"/>
+      <c r="AA14" s="13"/>
+      <c r="AB14" s="39"/>
     </row>
-    <row r="15" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M15" s="10"/>
-      <c r="N15" s="3"/>
-      <c r="O15" s="18"/>
-      <c r="P15" s="18"/>
-      <c r="Q15" s="18"/>
-      <c r="R15" s="18"/>
-      <c r="S15" s="8"/>
-      <c r="T15" s="8"/>
-      <c r="U15" s="8"/>
-      <c r="V15" s="8"/>
-      <c r="W15" s="8"/>
+    <row r="15" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D15" s="37"/>
+      <c r="E15" s="22"/>
+      <c r="F15" s="22"/>
+      <c r="G15" s="22"/>
+      <c r="H15" s="38"/>
+      <c r="I15" s="37"/>
+      <c r="J15" s="22" t="s">
+        <v>33</v>
+      </c>
+      <c r="K15" s="22"/>
+      <c r="L15" s="22"/>
+      <c r="M15" s="38"/>
+      <c r="N15" s="45"/>
+      <c r="O15" s="22" t="s">
+        <v>43</v>
+      </c>
+      <c r="P15" s="22"/>
+      <c r="Q15" s="22"/>
+      <c r="R15" s="38"/>
+      <c r="S15" s="37"/>
+      <c r="T15" s="29"/>
+      <c r="U15" s="29"/>
+      <c r="V15" s="29"/>
+      <c r="W15" s="46"/>
+      <c r="X15" s="37"/>
+      <c r="Y15" s="30"/>
+      <c r="Z15" s="30"/>
+      <c r="AA15" s="30"/>
+      <c r="AB15" s="49"/>
     </row>
-    <row r="16" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="M16" s="10"/>
-      <c r="N16" s="3"/>
-      <c r="O16" s="18"/>
-      <c r="P16" s="18"/>
-      <c r="Q16" s="18"/>
-      <c r="R16" s="18"/>
-      <c r="S16" s="8"/>
-      <c r="T16" s="8"/>
-      <c r="U16" s="8"/>
-      <c r="V16" s="8"/>
-      <c r="W16" s="8"/>
+    <row r="16" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D16" s="37"/>
+      <c r="E16" s="13"/>
+      <c r="F16" s="13"/>
+      <c r="G16" s="13"/>
+      <c r="H16" s="39"/>
+      <c r="I16" s="37"/>
+      <c r="J16" s="13"/>
+      <c r="K16" s="13"/>
+      <c r="L16" s="13"/>
+      <c r="M16" s="39"/>
+      <c r="N16" s="45"/>
+      <c r="O16" s="22" t="s">
+        <v>44</v>
+      </c>
+      <c r="P16" s="22"/>
+      <c r="Q16" s="22"/>
+      <c r="R16" s="38"/>
+      <c r="S16" s="37"/>
+      <c r="T16" s="31"/>
+      <c r="U16" s="31"/>
+      <c r="V16" s="31"/>
+      <c r="W16" s="47"/>
+      <c r="X16" s="37"/>
+      <c r="Y16" s="32"/>
+      <c r="Z16" s="32"/>
+      <c r="AA16" s="32"/>
+      <c r="AB16" s="50"/>
     </row>
-    <row r="17" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="A17" s="23" t="s">
+    <row r="17" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D17" s="37"/>
+      <c r="E17" s="13"/>
+      <c r="F17" s="13"/>
+      <c r="G17" s="13"/>
+      <c r="H17" s="39"/>
+      <c r="I17" s="37"/>
+      <c r="J17" s="13"/>
+      <c r="K17" s="13"/>
+      <c r="L17" s="13"/>
+      <c r="M17" s="39"/>
+      <c r="N17" s="45"/>
+      <c r="O17" s="22" t="s">
+        <v>45</v>
+      </c>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="38"/>
+      <c r="S17" s="37"/>
+      <c r="T17" s="31"/>
+      <c r="U17" s="31"/>
+      <c r="V17" s="31"/>
+      <c r="W17" s="47"/>
+      <c r="X17" s="37"/>
+      <c r="Y17" s="32"/>
+      <c r="Z17" s="32"/>
+      <c r="AA17" s="32"/>
+      <c r="AB17" s="50"/>
+    </row>
+    <row r="18" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D18" s="37"/>
+      <c r="E18" s="13"/>
+      <c r="F18" s="13"/>
+      <c r="G18" s="13"/>
+      <c r="H18" s="39"/>
+      <c r="I18" s="37"/>
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13"/>
+      <c r="M18" s="39"/>
+      <c r="N18" s="45"/>
+      <c r="O18" s="22" t="s">
+        <v>46</v>
+      </c>
+      <c r="P18" s="22"/>
+      <c r="Q18" s="22"/>
+      <c r="R18" s="38"/>
+      <c r="S18" s="37"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="47"/>
+      <c r="X18" s="37"/>
+      <c r="Y18" s="32"/>
+      <c r="Z18" s="32"/>
+      <c r="AA18" s="32"/>
+      <c r="AB18" s="50"/>
+    </row>
+    <row r="19" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D19" s="37"/>
+      <c r="E19" s="13"/>
+      <c r="F19" s="13"/>
+      <c r="G19" s="13"/>
+      <c r="H19" s="39"/>
+      <c r="I19" s="37"/>
+      <c r="J19" s="13"/>
+      <c r="K19" s="13"/>
+      <c r="L19" s="13"/>
+      <c r="M19" s="39"/>
+      <c r="N19" s="45"/>
+      <c r="O19" s="22" t="s">
+        <v>47</v>
+      </c>
+      <c r="P19" s="22"/>
+      <c r="Q19" s="22"/>
+      <c r="R19" s="38"/>
+      <c r="S19" s="37"/>
+      <c r="T19" s="31"/>
+      <c r="U19" s="31"/>
+      <c r="V19" s="31"/>
+      <c r="W19" s="47"/>
+      <c r="X19" s="37"/>
+      <c r="Y19" s="32"/>
+      <c r="Z19" s="32"/>
+      <c r="AA19" s="32"/>
+      <c r="AB19" s="50"/>
+    </row>
+    <row r="20" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D20" s="37"/>
+      <c r="E20" s="13"/>
+      <c r="F20" s="13"/>
+      <c r="G20" s="13"/>
+      <c r="H20" s="39"/>
+      <c r="I20" s="37"/>
+      <c r="J20" s="13"/>
+      <c r="K20" s="13"/>
+      <c r="L20" s="13"/>
+      <c r="M20" s="39"/>
+      <c r="N20" s="45"/>
+      <c r="O20" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="P20" s="22"/>
+      <c r="Q20" s="22"/>
+      <c r="R20" s="38"/>
+      <c r="S20" s="37"/>
+      <c r="T20" s="31"/>
+      <c r="U20" s="31"/>
+      <c r="V20" s="31"/>
+      <c r="W20" s="47"/>
+      <c r="X20" s="37"/>
+      <c r="Y20" s="32"/>
+      <c r="Z20" s="32"/>
+      <c r="AA20" s="32"/>
+      <c r="AB20" s="50"/>
+    </row>
+    <row r="21" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D21" s="37"/>
+      <c r="E21" s="13"/>
+      <c r="F21" s="13"/>
+      <c r="G21" s="13"/>
+      <c r="H21" s="39"/>
+      <c r="I21" s="37"/>
+      <c r="J21" s="13"/>
+      <c r="K21" s="13"/>
+      <c r="L21" s="13"/>
+      <c r="M21" s="39"/>
+      <c r="N21" s="45"/>
+      <c r="O21" s="22" t="s">
+        <v>49</v>
+      </c>
+      <c r="P21" s="22"/>
+      <c r="Q21" s="22"/>
+      <c r="R21" s="38"/>
+      <c r="S21" s="37"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="47"/>
+      <c r="X21" s="37"/>
+      <c r="Y21" s="32"/>
+      <c r="Z21" s="32"/>
+      <c r="AA21" s="32"/>
+      <c r="AB21" s="50"/>
+    </row>
+    <row r="22" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D22" s="37"/>
+      <c r="E22" s="13"/>
+      <c r="F22" s="13"/>
+      <c r="G22" s="13"/>
+      <c r="H22" s="39"/>
+      <c r="I22" s="37"/>
+      <c r="J22" s="13"/>
+      <c r="K22" s="13"/>
+      <c r="L22" s="13"/>
+      <c r="M22" s="39"/>
+      <c r="N22" s="45"/>
+      <c r="O22" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="P22" s="22"/>
+      <c r="Q22" s="22"/>
+      <c r="R22" s="38"/>
+      <c r="S22" s="37"/>
+      <c r="T22" s="31"/>
+      <c r="U22" s="31"/>
+      <c r="V22" s="31"/>
+      <c r="W22" s="47"/>
+      <c r="X22" s="37"/>
+      <c r="Y22" s="32"/>
+      <c r="Z22" s="32"/>
+      <c r="AA22" s="32"/>
+      <c r="AB22" s="50"/>
+    </row>
+    <row r="23" spans="1:28" ht="32.25" customHeight="1">
+      <c r="D23" s="37"/>
+      <c r="E23" s="14"/>
+      <c r="F23" s="14"/>
+      <c r="G23" s="14"/>
+      <c r="H23" s="40"/>
+      <c r="I23" s="37"/>
+      <c r="J23" s="14"/>
+      <c r="K23" s="14"/>
+      <c r="L23" s="14"/>
+      <c r="M23" s="40"/>
+      <c r="N23" s="45"/>
+      <c r="O23" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="38"/>
+      <c r="S23" s="37"/>
+      <c r="T23" s="15"/>
+      <c r="U23" s="15"/>
+      <c r="V23" s="15"/>
+      <c r="W23" s="48"/>
+      <c r="X23" s="37"/>
+      <c r="Y23" s="16"/>
+      <c r="Z23" s="16"/>
+      <c r="AA23" s="16"/>
+      <c r="AB23" s="51"/>
+    </row>
+    <row r="24" spans="1:28" ht="51.75" customHeight="1">
+      <c r="A24" s="23" t="s">
+        <v>20</v>
+      </c>
+      <c r="B24" s="23"/>
+      <c r="D24" s="24" t="s">
+        <v>21</v>
+      </c>
+      <c r="E24" s="25"/>
+      <c r="F24" s="25"/>
+      <c r="G24" s="25"/>
+      <c r="H24" s="26"/>
+      <c r="I24" s="24"/>
+      <c r="J24" s="25"/>
+      <c r="K24" s="25"/>
+      <c r="L24" s="25"/>
+      <c r="M24" s="26"/>
+      <c r="N24" s="24" t="s">
+        <v>34</v>
+      </c>
+      <c r="O24" s="25"/>
+      <c r="P24" s="25"/>
+      <c r="Q24" s="25"/>
+      <c r="R24" s="26"/>
+      <c r="S24" s="24"/>
+      <c r="T24" s="25"/>
+      <c r="U24" s="25"/>
+      <c r="V24" s="25"/>
+      <c r="W24" s="26"/>
+      <c r="X24" s="24"/>
+      <c r="Y24" s="25"/>
+      <c r="Z24" s="25"/>
+      <c r="AA24" s="25"/>
+      <c r="AB24" s="26"/>
+    </row>
+    <row r="25" spans="1:28" s="7" customFormat="1" ht="11.25" customHeight="1">
+      <c r="B25" s="9"/>
+      <c r="D25" s="10"/>
+      <c r="E25" s="10"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="10"/>
+      <c r="H25" s="10"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="11"/>
+      <c r="K25" s="11"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="11"/>
+      <c r="P25" s="11"/>
+      <c r="Q25" s="11"/>
+      <c r="R25" s="11"/>
+      <c r="S25" s="11"/>
+      <c r="T25" s="11"/>
+      <c r="U25" s="11"/>
+      <c r="V25" s="11"/>
+      <c r="W25" s="11"/>
+    </row>
+    <row r="26" spans="1:28" ht="15" customHeight="1">
+      <c r="M26" s="7"/>
+      <c r="N26" s="3"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="5"/>
+      <c r="T26" s="5"/>
+      <c r="U26" s="5"/>
+      <c r="V26" s="5"/>
+      <c r="W26" s="5"/>
+    </row>
+    <row r="27" spans="1:28" ht="15" customHeight="1">
+      <c r="M27" s="7"/>
+      <c r="N27" s="3"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="5"/>
+      <c r="T27" s="5"/>
+      <c r="U27" s="5"/>
+      <c r="V27" s="5"/>
+      <c r="W27" s="5"/>
+    </row>
+    <row r="28" spans="1:28">
+      <c r="A28" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="B17" s="23"/>
-      <c r="C17" s="17"/>
-      <c r="M17" s="10"/>
-      <c r="N17" s="10"/>
-      <c r="O17" s="11"/>
-      <c r="P17" s="11"/>
-      <c r="Q17" s="11"/>
-      <c r="R17" s="11"/>
-      <c r="S17" s="8"/>
-      <c r="T17" s="8"/>
-      <c r="U17" s="8"/>
-      <c r="V17" s="8"/>
-      <c r="W17" s="8"/>
+      <c r="B28" s="17"/>
+      <c r="C28" s="12"/>
+      <c r="M28" s="7"/>
+      <c r="N28" s="7"/>
+      <c r="O28" s="8"/>
+      <c r="P28" s="8"/>
+      <c r="Q28" s="8"/>
+      <c r="R28" s="8"/>
+      <c r="S28" s="5"/>
+      <c r="T28" s="5"/>
+      <c r="U28" s="5"/>
+      <c r="V28" s="5"/>
+      <c r="W28" s="5"/>
     </row>
-    <row r="18" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D18" s="2"/>
-      <c r="E18" s="2" t="s">
+    <row r="29" spans="1:28" ht="27" customHeight="1">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="O18" s="8"/>
-      <c r="P18" s="8"/>
-      <c r="Q18" s="8"/>
-      <c r="R18" s="8"/>
-      <c r="S18" s="9"/>
-      <c r="T18" s="9"/>
-      <c r="U18" s="8"/>
-      <c r="V18" s="18"/>
-      <c r="W18" s="18"/>
+      <c r="O29" s="5"/>
+      <c r="P29" s="5"/>
+      <c r="Q29" s="5"/>
+      <c r="R29" s="5"/>
+      <c r="S29" s="6"/>
+      <c r="T29" s="6"/>
+      <c r="U29" s="5"/>
+      <c r="V29" s="22"/>
+      <c r="W29" s="22"/>
     </row>
-    <row r="19" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D19" s="2"/>
-      <c r="E19" s="2" t="s">
+    <row r="30" spans="1:28" ht="27" customHeight="1">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="F19" s="2"/>
-      <c r="G19" s="2"/>
-      <c r="O19" s="8"/>
-      <c r="P19" s="8"/>
-      <c r="Q19" s="8"/>
-      <c r="R19" s="8"/>
-      <c r="S19" s="9"/>
-      <c r="T19" s="9"/>
-      <c r="U19" s="8"/>
-      <c r="V19" s="8"/>
-      <c r="W19" s="8"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="O30" s="5"/>
+      <c r="P30" s="5"/>
+      <c r="Q30" s="5"/>
+      <c r="R30" s="5"/>
+      <c r="S30" s="6"/>
+      <c r="T30" s="6"/>
+      <c r="U30" s="5"/>
+      <c r="V30" s="5"/>
+      <c r="W30" s="5"/>
     </row>
-    <row r="20" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E20" s="2" t="s">
+    <row r="31" spans="1:28" ht="27" customHeight="1">
+      <c r="E31" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="2"/>
-      <c r="O20" s="8"/>
-      <c r="P20" s="8"/>
-      <c r="Q20" s="8"/>
-      <c r="R20" s="8"/>
-      <c r="S20" s="8"/>
-      <c r="T20" s="8"/>
-      <c r="U20" s="8"/>
-      <c r="V20" s="8"/>
-      <c r="W20" s="8"/>
+      <c r="F31" s="2"/>
+      <c r="O31" s="5"/>
+      <c r="P31" s="5"/>
+      <c r="Q31" s="5"/>
+      <c r="R31" s="5"/>
+      <c r="S31" s="5"/>
+      <c r="T31" s="5"/>
+      <c r="U31" s="5"/>
+      <c r="V31" s="5"/>
+      <c r="W31" s="5"/>
     </row>
-    <row r="21" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E21" s="2" t="s">
+    <row r="32" spans="1:28" ht="27" customHeight="1">
+      <c r="E32" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="O21" s="8"/>
-      <c r="P21" s="8"/>
-      <c r="Q21" s="8"/>
-      <c r="R21" s="8"/>
-      <c r="S21" s="8"/>
-      <c r="T21" s="8"/>
-      <c r="U21" s="8"/>
-      <c r="V21" s="8"/>
-      <c r="W21" s="8"/>
+      <c r="O32" s="5"/>
+      <c r="P32" s="5"/>
+      <c r="Q32" s="5"/>
+      <c r="R32" s="5"/>
+      <c r="S32" s="5"/>
+      <c r="T32" s="5"/>
+      <c r="U32" s="5"/>
+      <c r="V32" s="5"/>
+      <c r="W32" s="5"/>
     </row>
-    <row r="22" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E22" s="2" t="s">
+    <row r="33" spans="5:23" ht="27" customHeight="1">
+      <c r="E33" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="F22" s="2"/>
-      <c r="O22" s="8"/>
-      <c r="P22" s="8"/>
-      <c r="Q22" s="8"/>
-      <c r="R22" s="8"/>
-      <c r="S22" s="8"/>
-      <c r="T22" s="8"/>
-      <c r="U22" s="8"/>
-      <c r="V22" s="8"/>
-      <c r="W22" s="8"/>
+      <c r="F33" s="2"/>
+      <c r="O33" s="5"/>
+      <c r="P33" s="5"/>
+      <c r="Q33" s="5"/>
+      <c r="R33" s="5"/>
+      <c r="S33" s="5"/>
+      <c r="T33" s="5"/>
+      <c r="U33" s="5"/>
+      <c r="V33" s="5"/>
+      <c r="W33" s="5"/>
     </row>
-    <row r="23" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E23" s="2" t="s">
+    <row r="34" spans="5:23" ht="27" customHeight="1">
+      <c r="E34" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="F23" s="2"/>
-      <c r="O23" s="8"/>
-      <c r="P23" s="8"/>
-      <c r="Q23" s="8"/>
-      <c r="R23" s="8"/>
-      <c r="S23" s="8"/>
-      <c r="T23" s="8"/>
-      <c r="U23" s="8"/>
-      <c r="V23" s="8"/>
-      <c r="W23" s="8"/>
+      <c r="F34" s="2"/>
+      <c r="O34" s="5"/>
+      <c r="P34" s="5"/>
+      <c r="Q34" s="5"/>
+      <c r="R34" s="5"/>
+      <c r="S34" s="5"/>
+      <c r="T34" s="5"/>
+      <c r="U34" s="5"/>
+      <c r="V34" s="5"/>
+      <c r="W34" s="5"/>
     </row>
-    <row r="24" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E24" s="2" t="s">
+    <row r="35" spans="5:23" ht="27" customHeight="1">
+      <c r="E35" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="F24" s="2"/>
-      <c r="O24" s="8"/>
-      <c r="P24" s="8"/>
-      <c r="Q24" s="8"/>
-      <c r="R24" s="8"/>
-      <c r="S24" s="8"/>
-      <c r="T24" s="8"/>
-      <c r="U24" s="8"/>
-      <c r="V24" s="8"/>
-      <c r="W24" s="8"/>
+      <c r="F35" s="2"/>
+      <c r="O35" s="5"/>
+      <c r="P35" s="5"/>
+      <c r="Q35" s="5"/>
+      <c r="R35" s="5"/>
+      <c r="S35" s="5"/>
+      <c r="T35" s="5"/>
+      <c r="U35" s="5"/>
+      <c r="V35" s="5"/>
+      <c r="W35" s="5"/>
     </row>
-    <row r="25" spans="1:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E25" s="2" t="s">
+    <row r="36" spans="5:23" ht="27" customHeight="1">
+      <c r="E36" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="F25" s="2"/>
-      <c r="O25" s="8"/>
-      <c r="P25" s="8"/>
-      <c r="Q25" s="8"/>
-      <c r="R25" s="8"/>
-      <c r="S25" s="8"/>
-      <c r="T25" s="8"/>
-      <c r="U25" s="8"/>
-      <c r="V25" s="8"/>
-      <c r="W25" s="8"/>
+      <c r="F36" s="2"/>
+      <c r="O36" s="5"/>
+      <c r="P36" s="5"/>
+      <c r="Q36" s="5"/>
+      <c r="R36" s="5"/>
+      <c r="S36" s="5"/>
+      <c r="T36" s="5"/>
+      <c r="U36" s="5"/>
+      <c r="V36" s="5"/>
+      <c r="W36" s="5"/>
     </row>
-    <row r="26" spans="1:23" x14ac:dyDescent="0.25">
-      <c r="E26" s="2"/>
-      <c r="F26" s="2"/>
+    <row r="37" spans="5:23">
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="47">
+  <mergeCells count="62">
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O16:R16"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="Y8:AB8"/>
+    <mergeCell ref="Y10:AB10"/>
+    <mergeCell ref="Y11:AB11"/>
+    <mergeCell ref="O26:R26"/>
+    <mergeCell ref="O27:R27"/>
+    <mergeCell ref="X24:AB24"/>
+    <mergeCell ref="Y9:AB9"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="I24:M24"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="S24:W24"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="T15:W15"/>
+    <mergeCell ref="Y15:AB15"/>
     <mergeCell ref="T7:W7"/>
     <mergeCell ref="Y7:AB7"/>
     <mergeCell ref="A4:B4"/>
@@ -2657,67 +3669,12 @@
     <mergeCell ref="J7:M7"/>
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="O7:R7"/>
-    <mergeCell ref="E12:H12"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="T12:W12"/>
-    <mergeCell ref="Y12:AB12"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="V18:W18"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="D13:H13"/>
-    <mergeCell ref="I13:M13"/>
-    <mergeCell ref="N13:R13"/>
-    <mergeCell ref="S13:W13"/>
-    <mergeCell ref="Y8:AB8"/>
-    <mergeCell ref="Y10:AB10"/>
-    <mergeCell ref="Y11:AB11"/>
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="O16:R16"/>
-    <mergeCell ref="X13:AB13"/>
-    <mergeCell ref="Y9:AB9"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J9:M9"/>
   </mergeCells>
-  <conditionalFormatting sqref="D6:R6 U6:W6">
-    <cfRule type="expression" dxfId="7" priority="7">
+  <conditionalFormatting sqref="D6:AB6">
+    <cfRule type="expression" dxfId="1" priority="7">
       <formula>AND(D6="H",ISNA(VLOOKUP(INDIRECT(ADDRESS(ROW(ProjectDays),COLUMN())),Holidays,1,FALSE)))</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="6" priority="8" operator="equal">
-      <formula>"H"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="S6:T6">
-    <cfRule type="expression" dxfId="5" priority="5">
-      <formula>AND(S6="H",ISNA(VLOOKUP(INDIRECT(ADDRESS(ROW(ProjectDays),COLUMN())),Holidays,1,FALSE)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
-      <formula>"H"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="Z6:AB6">
-    <cfRule type="expression" dxfId="3" priority="3">
-      <formula>AND(Z6="H",ISNA(VLOOKUP(INDIRECT(ADDRESS(ROW(ProjectDays),COLUMN())),Holidays,1,FALSE)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="4" operator="equal">
-      <formula>"H"</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="X6:Y6">
-    <cfRule type="expression" dxfId="1" priority="1">
-      <formula>AND(X6="H",ISNA(VLOOKUP(INDIRECT(ADDRESS(ROW(ProjectDays),COLUMN())),Holidays,1,FALSE)))</formula>
-    </cfRule>
-    <cfRule type="cellIs" dxfId="0" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="8" operator="equal">
       <formula>"H"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
# Updated delivery map
</commit_message>
<xml_diff>
--- a/docs/MapaEntregables.xlsx
+++ b/docs/MapaEntregables.xlsx
@@ -1,8 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr updateLinks="always" codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian\Documents\UBA\2do Cuat 2013\TallerDesarrollo2\docs\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="8235"/>
   </bookViews>
@@ -53,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
   <si>
     <t>Code/Implementation</t>
   </si>
@@ -206,18 +211,33 @@
   </si>
   <si>
     <t>Ver Cartelera de Complejo</t>
+  </si>
+  <si>
+    <t>Compra de entradas</t>
+  </si>
+  <si>
+    <t>Reserva de entradas</t>
+  </si>
+  <si>
+    <t>Listado de reservas y compras de un usuario</t>
+  </si>
+  <si>
+    <t>Cargar disposición física de sala a partir de un archivo</t>
+  </si>
+  <si>
+    <t>Administración de promociones</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="_-* #,##0.00\ _€_-;\-* #,##0.00\ _€_-;_-* &quot;-&quot;??\ _€_-;_-@_-"/>
     <numFmt numFmtId="165" formatCode="[$-409]d\-mmm\-yy;@"/>
     <numFmt numFmtId="166" formatCode="&quot;Iteration&quot;\ 0"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -304,20 +324,11 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="12">
     <border>
       <left/>
       <right/>
       <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
       <bottom/>
       <diagonal/>
     </border>
@@ -356,17 +367,6 @@
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color auto="1"/>
-      </right>
-      <top style="thin">
-        <color theme="1"/>
-      </top>
-      <bottom/>
       <diagonal/>
     </border>
     <border>
@@ -454,7 +454,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -463,7 +463,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
@@ -485,117 +485,108 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1016,7 +1007,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6434172" y="1932191"/>
+          <a:off x="7367355" y="1932191"/>
           <a:ext cx="214312" cy="227009"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1370,20 +1361,20 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>43961</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>58614</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>258274</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>291180</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="42" name="Picture 41" descr="document_text_32.png"/>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>87923</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>65943</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>302236</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>298509</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="43" name="Picture 42" descr="document_text_32.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1396,7 +1387,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="6740769" y="2256691"/>
+          <a:off x="8264769" y="1208943"/>
           <a:ext cx="214313" cy="232566"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1414,18 +1405,18 @@
     <xdr:from>
       <xdr:col>23</xdr:col>
       <xdr:colOff>87923</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>65943</xdr:rowOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>43962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
       <xdr:colOff>302236</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>298509</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="Picture 42" descr="document_text_32.png"/>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>276528</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="45" name="Picture 44" descr="document_text_32.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1438,7 +1429,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8264769" y="1208943"/>
+          <a:off x="8264769" y="1567962"/>
           <a:ext cx="214313" cy="232566"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1455,19 +1446,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>87923</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>43962</xdr:rowOff>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>302236</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>276528</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="45" name="Picture 44" descr="document_text_32.png"/>
+      <xdr:colOff>309563</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>239893</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="46" name="Picture 45" descr="document_text_32.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1480,7 +1471,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8264769" y="1567962"/>
+          <a:off x="8272096" y="1912327"/>
           <a:ext cx="214313" cy="232566"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1497,19 +1488,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7327</xdr:rowOff>
+      <xdr:colOff>95249</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>43962</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>309563</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>239893</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="46" name="Picture 45" descr="document_text_32.png"/>
+      <xdr:colOff>309562</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>276528</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="47" name="Picture 46" descr="document_text_32.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1522,7 +1513,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8272096" y="1912327"/>
+          <a:off x="8272095" y="2242039"/>
           <a:ext cx="214313" cy="232566"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1539,19 +1530,19 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>43962</xdr:rowOff>
+      <xdr:colOff>87923</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>7327</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>23</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>276528</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Picture 46" descr="document_text_32.png"/>
+      <xdr:colOff>302236</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>239893</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="49" name="Picture 48" descr="document_text_32.png"/>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1"/>
         </xdr:cNvPicPr>
@@ -1564,7 +1555,7 @@
       </xdr:blipFill>
       <xdr:spPr>
         <a:xfrm>
-          <a:off x="8272095" y="2242039"/>
+          <a:off x="8264769" y="2586404"/>
           <a:ext cx="214313" cy="232566"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1580,48 +1571,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>87923</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>7327</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>302236</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>239893</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Picture 48" descr="document_text_32.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8264769" y="2586404"/>
-          <a:ext cx="214313" cy="232566"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>14653</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -2418,11 +2367,87 @@
     </xdr:pic>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>43295</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>51954</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>257607</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>278963</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="48" name="Picture 47" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7394863" y="2251363"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>51954</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>43295</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>266266</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>270304</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="50" name="Picture 49" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="7403522" y="2623704"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
   <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
     <sheetNames>
       <sheetName val="w-plan"/>
@@ -2453,7 +2478,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2495,7 +2520,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2527,9 +2552,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2561,6 +2587,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -2736,14 +2763,14 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A4:AB37"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C22" zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4:R24"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="90" workbookViewId="0">
+      <selection activeCell="S24" sqref="A4:W24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="5.85546875" style="1" customWidth="1"/>
     <col min="2" max="2" width="11.28515625" style="1" customWidth="1"/>
@@ -2756,664 +2783,674 @@
     <col min="55" max="16384" width="8.85546875" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="1:28">
-      <c r="A4" s="17" t="s">
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="35" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="17"/>
-      <c r="D4" s="33" t="s">
+      <c r="B4" s="35"/>
+      <c r="D4" s="41" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="34"/>
-      <c r="F4" s="34"/>
-      <c r="G4" s="34"/>
-      <c r="H4" s="35"/>
-      <c r="I4" s="18" t="s">
+      <c r="E4" s="42"/>
+      <c r="F4" s="42"/>
+      <c r="G4" s="42"/>
+      <c r="H4" s="43"/>
+      <c r="I4" s="41" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="18"/>
-      <c r="K4" s="18"/>
-      <c r="L4" s="18"/>
-      <c r="M4" s="19"/>
-      <c r="N4" s="33" t="s">
+      <c r="J4" s="42"/>
+      <c r="K4" s="42"/>
+      <c r="L4" s="42"/>
+      <c r="M4" s="43"/>
+      <c r="N4" s="41" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="34"/>
-      <c r="P4" s="34"/>
-      <c r="Q4" s="34"/>
-      <c r="R4" s="35"/>
-      <c r="S4" s="33" t="s">
+      <c r="O4" s="42"/>
+      <c r="P4" s="42"/>
+      <c r="Q4" s="42"/>
+      <c r="R4" s="43"/>
+      <c r="S4" s="41" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="34"/>
-      <c r="U4" s="34"/>
-      <c r="V4" s="34"/>
-      <c r="W4" s="35"/>
-      <c r="X4" s="33" t="s">
+      <c r="T4" s="42"/>
+      <c r="U4" s="42"/>
+      <c r="V4" s="42"/>
+      <c r="W4" s="43"/>
+      <c r="X4" s="41" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" s="34"/>
-      <c r="Z4" s="34"/>
-      <c r="AA4" s="34"/>
-      <c r="AB4" s="35"/>
+      <c r="Y4" s="42"/>
+      <c r="Z4" s="42"/>
+      <c r="AA4" s="42"/>
+      <c r="AB4" s="43"/>
     </row>
-    <row r="5" spans="1:28">
-      <c r="D5" s="36" t="s">
+    <row r="5" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="D5" s="44" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="20"/>
-      <c r="F5" s="20"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="21"/>
-      <c r="I5" s="41" t="s">
+      <c r="E5" s="45"/>
+      <c r="F5" s="45"/>
+      <c r="G5" s="45"/>
+      <c r="H5" s="46"/>
+      <c r="I5" s="44" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="43"/>
-      <c r="N5" s="36" t="s">
+      <c r="J5" s="45"/>
+      <c r="K5" s="45"/>
+      <c r="L5" s="45"/>
+      <c r="M5" s="46"/>
+      <c r="N5" s="44" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="20"/>
-      <c r="P5" s="20"/>
-      <c r="Q5" s="20"/>
-      <c r="R5" s="21"/>
-      <c r="S5" s="36" t="s">
+      <c r="O5" s="45"/>
+      <c r="P5" s="45"/>
+      <c r="Q5" s="45"/>
+      <c r="R5" s="46"/>
+      <c r="S5" s="44" t="s">
         <v>23</v>
       </c>
-      <c r="T5" s="20"/>
-      <c r="U5" s="20"/>
-      <c r="V5" s="20"/>
-      <c r="W5" s="21"/>
-      <c r="X5" s="36" t="s">
+      <c r="T5" s="45"/>
+      <c r="U5" s="45"/>
+      <c r="V5" s="45"/>
+      <c r="W5" s="46"/>
+      <c r="X5" s="44" t="s">
         <v>24</v>
       </c>
-      <c r="Y5" s="20"/>
-      <c r="Z5" s="20"/>
-      <c r="AA5" s="20"/>
-      <c r="AB5" s="21"/>
+      <c r="Y5" s="45"/>
+      <c r="Z5" s="45"/>
+      <c r="AA5" s="45"/>
+      <c r="AB5" s="46"/>
     </row>
-    <row r="6" spans="1:28">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
-      <c r="E6" s="27"/>
-      <c r="F6" s="27"/>
-      <c r="G6" s="27"/>
-      <c r="H6" s="28"/>
-      <c r="I6" s="44"/>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27"/>
-      <c r="L6" s="27"/>
-      <c r="M6" s="28"/>
-      <c r="N6" s="44"/>
-      <c r="O6" s="27"/>
-      <c r="P6" s="27"/>
-      <c r="Q6" s="27"/>
-      <c r="R6" s="28"/>
-      <c r="S6" s="44"/>
-      <c r="T6" s="27"/>
-      <c r="U6" s="27"/>
-      <c r="V6" s="27"/>
-      <c r="W6" s="28"/>
-      <c r="X6" s="44"/>
-      <c r="Y6" s="27"/>
-      <c r="Z6" s="27"/>
-      <c r="AA6" s="27"/>
-      <c r="AB6" s="28"/>
+      <c r="E6" s="17"/>
+      <c r="F6" s="17"/>
+      <c r="G6" s="17"/>
+      <c r="H6" s="18"/>
+      <c r="I6" s="24"/>
+      <c r="J6" s="17"/>
+      <c r="K6" s="17"/>
+      <c r="L6" s="17"/>
+      <c r="M6" s="18"/>
+      <c r="N6" s="24"/>
+      <c r="O6" s="17"/>
+      <c r="P6" s="17"/>
+      <c r="Q6" s="17"/>
+      <c r="R6" s="18"/>
+      <c r="S6" s="24"/>
+      <c r="T6" s="17"/>
+      <c r="U6" s="17"/>
+      <c r="V6" s="17"/>
+      <c r="W6" s="18"/>
+      <c r="X6" s="24"/>
+      <c r="Y6" s="17"/>
+      <c r="Z6" s="17"/>
+      <c r="AA6" s="17"/>
+      <c r="AB6" s="18"/>
     </row>
-    <row r="7" spans="1:28" ht="30" customHeight="1">
-      <c r="D7" s="37"/>
-      <c r="E7" s="22" t="s">
+    <row r="7" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D7" s="21"/>
+      <c r="E7" s="30" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="22"/>
-      <c r="G7" s="22"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="37"/>
-      <c r="J7" s="22" t="s">
+      <c r="F7" s="30"/>
+      <c r="G7" s="30"/>
+      <c r="H7" s="31"/>
+      <c r="I7" s="21"/>
+      <c r="J7" s="30" t="s">
         <v>27</v>
       </c>
-      <c r="K7" s="22"/>
-      <c r="L7" s="22"/>
-      <c r="M7" s="38"/>
-      <c r="N7" s="37"/>
-      <c r="O7" s="22" t="s">
+      <c r="K7" s="30"/>
+      <c r="L7" s="30"/>
+      <c r="M7" s="31"/>
+      <c r="N7" s="21"/>
+      <c r="O7" s="30" t="s">
         <v>35</v>
       </c>
-      <c r="P7" s="22"/>
-      <c r="Q7" s="22"/>
-      <c r="R7" s="38"/>
-      <c r="S7" s="37"/>
-      <c r="T7" s="22"/>
-      <c r="U7" s="22"/>
-      <c r="V7" s="22"/>
-      <c r="W7" s="38"/>
-      <c r="X7" s="37"/>
-      <c r="Y7" s="22"/>
-      <c r="Z7" s="22"/>
-      <c r="AA7" s="22"/>
-      <c r="AB7" s="38"/>
+      <c r="P7" s="30"/>
+      <c r="Q7" s="30"/>
+      <c r="R7" s="31"/>
+      <c r="S7" s="21"/>
+      <c r="T7" s="30" t="s">
+        <v>51</v>
+      </c>
+      <c r="U7" s="30"/>
+      <c r="V7" s="30"/>
+      <c r="W7" s="31"/>
+      <c r="X7" s="21"/>
+      <c r="Y7" s="30"/>
+      <c r="Z7" s="30"/>
+      <c r="AA7" s="30"/>
+      <c r="AB7" s="31"/>
     </row>
-    <row r="8" spans="1:28" ht="30" customHeight="1">
-      <c r="D8" s="37"/>
-      <c r="E8" s="22" t="s">
+    <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D8" s="21"/>
+      <c r="E8" s="30" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="22"/>
-      <c r="G8" s="22"/>
-      <c r="H8" s="38"/>
-      <c r="I8" s="37"/>
-      <c r="J8" s="22" t="s">
+      <c r="F8" s="30"/>
+      <c r="G8" s="30"/>
+      <c r="H8" s="31"/>
+      <c r="I8" s="21"/>
+      <c r="J8" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="K8" s="22"/>
-      <c r="L8" s="22"/>
-      <c r="M8" s="38"/>
-      <c r="N8" s="45"/>
-      <c r="O8" s="22" t="s">
+      <c r="K8" s="30"/>
+      <c r="L8" s="30"/>
+      <c r="M8" s="31"/>
+      <c r="N8" s="25"/>
+      <c r="O8" s="30" t="s">
         <v>36</v>
       </c>
-      <c r="P8" s="22"/>
-      <c r="Q8" s="22"/>
-      <c r="R8" s="38"/>
-      <c r="S8" s="37"/>
-      <c r="T8" s="22"/>
-      <c r="U8" s="22"/>
-      <c r="V8" s="22"/>
-      <c r="W8" s="38"/>
-      <c r="X8" s="37"/>
-      <c r="Y8" s="22"/>
-      <c r="Z8" s="22"/>
-      <c r="AA8" s="22"/>
-      <c r="AB8" s="38"/>
+      <c r="P8" s="30"/>
+      <c r="Q8" s="30"/>
+      <c r="R8" s="31"/>
+      <c r="S8" s="21"/>
+      <c r="T8" s="30" t="s">
+        <v>52</v>
+      </c>
+      <c r="U8" s="30"/>
+      <c r="V8" s="30"/>
+      <c r="W8" s="31"/>
+      <c r="X8" s="21"/>
+      <c r="Y8" s="30"/>
+      <c r="Z8" s="30"/>
+      <c r="AA8" s="30"/>
+      <c r="AB8" s="31"/>
     </row>
-    <row r="9" spans="1:28" ht="23.25" customHeight="1">
-      <c r="D9" s="37"/>
-      <c r="E9" s="22" t="s">
+    <row r="9" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D9" s="21"/>
+      <c r="E9" s="30" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="22"/>
-      <c r="G9" s="22"/>
-      <c r="H9" s="38"/>
-      <c r="I9" s="37"/>
-      <c r="J9" s="22" t="s">
+      <c r="F9" s="30"/>
+      <c r="G9" s="30"/>
+      <c r="H9" s="31"/>
+      <c r="I9" s="21"/>
+      <c r="J9" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="K9" s="22"/>
-      <c r="L9" s="22"/>
-      <c r="M9" s="38"/>
-      <c r="N9" s="45"/>
-      <c r="O9" s="22" t="s">
+      <c r="K9" s="30"/>
+      <c r="L9" s="30"/>
+      <c r="M9" s="31"/>
+      <c r="N9" s="25"/>
+      <c r="O9" s="30" t="s">
         <v>37</v>
       </c>
-      <c r="P9" s="22"/>
-      <c r="Q9" s="22"/>
-      <c r="R9" s="38"/>
-      <c r="S9" s="37"/>
-      <c r="T9" s="22"/>
-      <c r="U9" s="22"/>
-      <c r="V9" s="22"/>
-      <c r="W9" s="38"/>
-      <c r="X9" s="37"/>
-      <c r="Y9" s="22"/>
-      <c r="Z9" s="22"/>
-      <c r="AA9" s="22"/>
-      <c r="AB9" s="38"/>
+      <c r="P9" s="30"/>
+      <c r="Q9" s="30"/>
+      <c r="R9" s="31"/>
+      <c r="S9" s="21"/>
+      <c r="T9" s="30" t="s">
+        <v>53</v>
+      </c>
+      <c r="U9" s="30"/>
+      <c r="V9" s="30"/>
+      <c r="W9" s="31"/>
+      <c r="X9" s="21"/>
+      <c r="Y9" s="30"/>
+      <c r="Z9" s="30"/>
+      <c r="AA9" s="30"/>
+      <c r="AB9" s="31"/>
     </row>
-    <row r="10" spans="1:28" ht="30" customHeight="1">
-      <c r="D10" s="37"/>
+    <row r="10" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D10" s="21"/>
       <c r="E10" s="13"/>
       <c r="F10" s="13"/>
       <c r="G10" s="13"/>
-      <c r="H10" s="39"/>
-      <c r="I10" s="37"/>
-      <c r="J10" s="22" t="s">
+      <c r="H10" s="22"/>
+      <c r="I10" s="21"/>
+      <c r="J10" s="30" t="s">
         <v>28</v>
       </c>
-      <c r="K10" s="22"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="38"/>
-      <c r="N10" s="45"/>
-      <c r="O10" s="22" t="s">
+      <c r="K10" s="30"/>
+      <c r="L10" s="30"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="25"/>
+      <c r="O10" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="P10" s="22"/>
-      <c r="Q10" s="22"/>
-      <c r="R10" s="38"/>
-      <c r="S10" s="37"/>
-      <c r="T10" s="22"/>
-      <c r="U10" s="22"/>
-      <c r="V10" s="22"/>
-      <c r="W10" s="38"/>
-      <c r="X10" s="37"/>
-      <c r="Y10" s="22"/>
-      <c r="Z10" s="22"/>
-      <c r="AA10" s="22"/>
-      <c r="AB10" s="38"/>
+      <c r="P10" s="30"/>
+      <c r="Q10" s="30"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="21"/>
+      <c r="T10" s="47" t="s">
+        <v>54</v>
+      </c>
+      <c r="U10" s="47"/>
+      <c r="V10" s="47"/>
+      <c r="W10" s="48"/>
+      <c r="X10" s="21"/>
+      <c r="Y10" s="30"/>
+      <c r="Z10" s="30"/>
+      <c r="AA10" s="30"/>
+      <c r="AB10" s="31"/>
     </row>
-    <row r="11" spans="1:28" ht="30.75" customHeight="1">
-      <c r="D11" s="37"/>
+    <row r="11" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D11" s="21"/>
       <c r="E11" s="13"/>
       <c r="F11" s="13"/>
       <c r="G11" s="13"/>
-      <c r="H11" s="39"/>
-      <c r="I11" s="37"/>
-      <c r="J11" s="22" t="s">
+      <c r="H11" s="22"/>
+      <c r="I11" s="21"/>
+      <c r="J11" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="K11" s="22"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="38"/>
-      <c r="N11" s="45"/>
-      <c r="O11" s="22" t="s">
+      <c r="K11" s="30"/>
+      <c r="L11" s="30"/>
+      <c r="M11" s="31"/>
+      <c r="N11" s="25"/>
+      <c r="O11" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="P11" s="22"/>
-      <c r="Q11" s="22"/>
-      <c r="R11" s="38"/>
-      <c r="S11" s="37"/>
-      <c r="T11" s="13"/>
-      <c r="U11" s="13"/>
-      <c r="V11" s="13"/>
-      <c r="W11" s="39"/>
-      <c r="X11" s="37"/>
-      <c r="Y11" s="22"/>
-      <c r="Z11" s="22"/>
-      <c r="AA11" s="22"/>
-      <c r="AB11" s="38"/>
+      <c r="P11" s="30"/>
+      <c r="Q11" s="30"/>
+      <c r="R11" s="31"/>
+      <c r="S11" s="21"/>
+      <c r="T11" s="30" t="s">
+        <v>55</v>
+      </c>
+      <c r="U11" s="30"/>
+      <c r="V11" s="30"/>
+      <c r="W11" s="31"/>
+      <c r="X11" s="21"/>
+      <c r="Y11" s="30"/>
+      <c r="Z11" s="30"/>
+      <c r="AA11" s="30"/>
+      <c r="AB11" s="31"/>
     </row>
-    <row r="12" spans="1:28" ht="28.5" customHeight="1">
-      <c r="D12" s="37"/>
+    <row r="12" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D12" s="21"/>
       <c r="E12" s="13"/>
       <c r="F12" s="13"/>
       <c r="G12" s="13"/>
-      <c r="H12" s="39"/>
-      <c r="I12" s="37"/>
-      <c r="J12" s="22" t="s">
+      <c r="H12" s="22"/>
+      <c r="I12" s="21"/>
+      <c r="J12" s="30" t="s">
         <v>30</v>
       </c>
-      <c r="K12" s="22"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="38"/>
-      <c r="N12" s="45"/>
-      <c r="O12" s="22" t="s">
+      <c r="K12" s="30"/>
+      <c r="L12" s="30"/>
+      <c r="M12" s="31"/>
+      <c r="N12" s="25"/>
+      <c r="O12" s="30" t="s">
         <v>40</v>
       </c>
-      <c r="P12" s="22"/>
-      <c r="Q12" s="22"/>
-      <c r="R12" s="38"/>
-      <c r="S12" s="37"/>
+      <c r="P12" s="30"/>
+      <c r="Q12" s="30"/>
+      <c r="R12" s="31"/>
+      <c r="S12" s="21"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
       <c r="V12" s="13"/>
-      <c r="W12" s="39"/>
-      <c r="X12" s="37"/>
+      <c r="W12" s="22"/>
+      <c r="X12" s="21"/>
       <c r="Y12" s="13"/>
       <c r="Z12" s="13"/>
       <c r="AA12" s="13"/>
-      <c r="AB12" s="39"/>
+      <c r="AB12" s="22"/>
     </row>
-    <row r="13" spans="1:28" ht="30.75" customHeight="1">
-      <c r="D13" s="37"/>
+    <row r="13" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D13" s="21"/>
       <c r="E13" s="13"/>
       <c r="F13" s="13"/>
       <c r="G13" s="13"/>
-      <c r="H13" s="39"/>
-      <c r="I13" s="37"/>
-      <c r="J13" s="22" t="s">
+      <c r="H13" s="22"/>
+      <c r="I13" s="21"/>
+      <c r="J13" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="K13" s="22"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="38"/>
-      <c r="N13" s="37"/>
-      <c r="O13" s="22" t="s">
+      <c r="K13" s="30"/>
+      <c r="L13" s="30"/>
+      <c r="M13" s="31"/>
+      <c r="N13" s="21"/>
+      <c r="O13" s="30" t="s">
         <v>41</v>
       </c>
-      <c r="P13" s="22"/>
-      <c r="Q13" s="22"/>
-      <c r="R13" s="38"/>
-      <c r="S13" s="37"/>
+      <c r="P13" s="30"/>
+      <c r="Q13" s="30"/>
+      <c r="R13" s="31"/>
+      <c r="S13" s="21"/>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
       <c r="V13" s="13"/>
-      <c r="W13" s="39"/>
-      <c r="X13" s="37"/>
+      <c r="W13" s="22"/>
+      <c r="X13" s="21"/>
       <c r="Y13" s="13"/>
       <c r="Z13" s="13"/>
       <c r="AA13" s="13"/>
-      <c r="AB13" s="39"/>
+      <c r="AB13" s="22"/>
     </row>
-    <row r="14" spans="1:28" ht="24" customHeight="1">
-      <c r="D14" s="37"/>
+    <row r="14" spans="1:28" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D14" s="21"/>
       <c r="E14" s="13"/>
       <c r="F14" s="13"/>
       <c r="G14" s="13"/>
-      <c r="H14" s="39"/>
-      <c r="I14" s="37"/>
-      <c r="J14" s="22" t="s">
+      <c r="H14" s="22"/>
+      <c r="I14" s="21"/>
+      <c r="J14" s="30" t="s">
         <v>32</v>
       </c>
-      <c r="K14" s="22"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="38"/>
-      <c r="N14" s="37"/>
-      <c r="O14" s="22" t="s">
+      <c r="K14" s="30"/>
+      <c r="L14" s="30"/>
+      <c r="M14" s="31"/>
+      <c r="N14" s="21"/>
+      <c r="O14" s="30" t="s">
         <v>42</v>
       </c>
-      <c r="P14" s="22"/>
-      <c r="Q14" s="22"/>
-      <c r="R14" s="38"/>
-      <c r="S14" s="37"/>
+      <c r="P14" s="30"/>
+      <c r="Q14" s="30"/>
+      <c r="R14" s="31"/>
+      <c r="S14" s="21"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
       <c r="V14" s="13"/>
-      <c r="W14" s="39"/>
-      <c r="X14" s="37"/>
+      <c r="W14" s="22"/>
+      <c r="X14" s="21"/>
       <c r="Y14" s="13"/>
       <c r="Z14" s="13"/>
       <c r="AA14" s="13"/>
-      <c r="AB14" s="39"/>
+      <c r="AB14" s="22"/>
     </row>
-    <row r="15" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D15" s="37"/>
-      <c r="E15" s="22"/>
-      <c r="F15" s="22"/>
-      <c r="G15" s="22"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="37"/>
-      <c r="J15" s="22" t="s">
+    <row r="15" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D15" s="21"/>
+      <c r="E15" s="30"/>
+      <c r="F15" s="30"/>
+      <c r="G15" s="30"/>
+      <c r="H15" s="31"/>
+      <c r="I15" s="21"/>
+      <c r="J15" s="30" t="s">
         <v>33</v>
       </c>
-      <c r="K15" s="22"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="38"/>
-      <c r="N15" s="45"/>
-      <c r="O15" s="22" t="s">
+      <c r="K15" s="30"/>
+      <c r="L15" s="30"/>
+      <c r="M15" s="31"/>
+      <c r="N15" s="25"/>
+      <c r="O15" s="30" t="s">
         <v>43</v>
       </c>
-      <c r="P15" s="22"/>
-      <c r="Q15" s="22"/>
-      <c r="R15" s="38"/>
-      <c r="S15" s="37"/>
-      <c r="T15" s="29"/>
-      <c r="U15" s="29"/>
-      <c r="V15" s="29"/>
-      <c r="W15" s="46"/>
-      <c r="X15" s="37"/>
-      <c r="Y15" s="30"/>
-      <c r="Z15" s="30"/>
-      <c r="AA15" s="30"/>
-      <c r="AB15" s="49"/>
+      <c r="P15" s="30"/>
+      <c r="Q15" s="30"/>
+      <c r="R15" s="31"/>
+      <c r="S15" s="21"/>
+      <c r="T15" s="37"/>
+      <c r="U15" s="37"/>
+      <c r="V15" s="37"/>
+      <c r="W15" s="38"/>
+      <c r="X15" s="21"/>
+      <c r="Y15" s="39"/>
+      <c r="Z15" s="39"/>
+      <c r="AA15" s="39"/>
+      <c r="AB15" s="40"/>
     </row>
-    <row r="16" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D16" s="37"/>
+    <row r="16" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D16" s="21"/>
       <c r="E16" s="13"/>
       <c r="F16" s="13"/>
       <c r="G16" s="13"/>
-      <c r="H16" s="39"/>
-      <c r="I16" s="37"/>
+      <c r="H16" s="22"/>
+      <c r="I16" s="21"/>
       <c r="J16" s="13"/>
       <c r="K16" s="13"/>
       <c r="L16" s="13"/>
-      <c r="M16" s="39"/>
-      <c r="N16" s="45"/>
-      <c r="O16" s="22" t="s">
+      <c r="M16" s="22"/>
+      <c r="N16" s="25"/>
+      <c r="O16" s="30" t="s">
         <v>44</v>
       </c>
-      <c r="P16" s="22"/>
-      <c r="Q16" s="22"/>
-      <c r="R16" s="38"/>
-      <c r="S16" s="37"/>
-      <c r="T16" s="31"/>
-      <c r="U16" s="31"/>
-      <c r="V16" s="31"/>
-      <c r="W16" s="47"/>
-      <c r="X16" s="37"/>
-      <c r="Y16" s="32"/>
-      <c r="Z16" s="32"/>
-      <c r="AA16" s="32"/>
-      <c r="AB16" s="50"/>
+      <c r="P16" s="30"/>
+      <c r="Q16" s="30"/>
+      <c r="R16" s="31"/>
+      <c r="S16" s="21"/>
+      <c r="T16" s="19"/>
+      <c r="U16" s="19"/>
+      <c r="V16" s="19"/>
+      <c r="W16" s="26"/>
+      <c r="X16" s="21"/>
+      <c r="Y16" s="20"/>
+      <c r="Z16" s="20"/>
+      <c r="AA16" s="20"/>
+      <c r="AB16" s="28"/>
     </row>
-    <row r="17" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D17" s="37"/>
+    <row r="17" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D17" s="21"/>
       <c r="E17" s="13"/>
       <c r="F17" s="13"/>
       <c r="G17" s="13"/>
-      <c r="H17" s="39"/>
-      <c r="I17" s="37"/>
+      <c r="H17" s="22"/>
+      <c r="I17" s="21"/>
       <c r="J17" s="13"/>
       <c r="K17" s="13"/>
       <c r="L17" s="13"/>
-      <c r="M17" s="39"/>
-      <c r="N17" s="45"/>
-      <c r="O17" s="22" t="s">
+      <c r="M17" s="22"/>
+      <c r="N17" s="25"/>
+      <c r="O17" s="30" t="s">
         <v>45</v>
       </c>
-      <c r="P17" s="22"/>
-      <c r="Q17" s="22"/>
-      <c r="R17" s="38"/>
-      <c r="S17" s="37"/>
-      <c r="T17" s="31"/>
-      <c r="U17" s="31"/>
-      <c r="V17" s="31"/>
-      <c r="W17" s="47"/>
-      <c r="X17" s="37"/>
-      <c r="Y17" s="32"/>
-      <c r="Z17" s="32"/>
-      <c r="AA17" s="32"/>
-      <c r="AB17" s="50"/>
+      <c r="P17" s="30"/>
+      <c r="Q17" s="30"/>
+      <c r="R17" s="31"/>
+      <c r="S17" s="21"/>
+      <c r="T17" s="19"/>
+      <c r="U17" s="19"/>
+      <c r="V17" s="19"/>
+      <c r="W17" s="26"/>
+      <c r="X17" s="21"/>
+      <c r="Y17" s="20"/>
+      <c r="Z17" s="20"/>
+      <c r="AA17" s="20"/>
+      <c r="AB17" s="28"/>
     </row>
-    <row r="18" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D18" s="37"/>
+    <row r="18" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D18" s="21"/>
       <c r="E18" s="13"/>
       <c r="F18" s="13"/>
       <c r="G18" s="13"/>
-      <c r="H18" s="39"/>
-      <c r="I18" s="37"/>
+      <c r="H18" s="22"/>
+      <c r="I18" s="21"/>
       <c r="J18" s="13"/>
       <c r="K18" s="13"/>
       <c r="L18" s="13"/>
-      <c r="M18" s="39"/>
-      <c r="N18" s="45"/>
-      <c r="O18" s="22" t="s">
+      <c r="M18" s="22"/>
+      <c r="N18" s="25"/>
+      <c r="O18" s="30" t="s">
         <v>46</v>
       </c>
-      <c r="P18" s="22"/>
-      <c r="Q18" s="22"/>
-      <c r="R18" s="38"/>
-      <c r="S18" s="37"/>
-      <c r="T18" s="31"/>
-      <c r="U18" s="31"/>
-      <c r="V18" s="31"/>
-      <c r="W18" s="47"/>
-      <c r="X18" s="37"/>
-      <c r="Y18" s="32"/>
-      <c r="Z18" s="32"/>
-      <c r="AA18" s="32"/>
-      <c r="AB18" s="50"/>
+      <c r="P18" s="30"/>
+      <c r="Q18" s="30"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="21"/>
+      <c r="T18" s="19"/>
+      <c r="U18" s="19"/>
+      <c r="V18" s="19"/>
+      <c r="W18" s="26"/>
+      <c r="X18" s="21"/>
+      <c r="Y18" s="20"/>
+      <c r="Z18" s="20"/>
+      <c r="AA18" s="20"/>
+      <c r="AB18" s="28"/>
     </row>
-    <row r="19" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D19" s="37"/>
+    <row r="19" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D19" s="21"/>
       <c r="E19" s="13"/>
       <c r="F19" s="13"/>
       <c r="G19" s="13"/>
-      <c r="H19" s="39"/>
-      <c r="I19" s="37"/>
+      <c r="H19" s="22"/>
+      <c r="I19" s="21"/>
       <c r="J19" s="13"/>
       <c r="K19" s="13"/>
       <c r="L19" s="13"/>
-      <c r="M19" s="39"/>
-      <c r="N19" s="45"/>
-      <c r="O19" s="22" t="s">
+      <c r="M19" s="22"/>
+      <c r="N19" s="25"/>
+      <c r="O19" s="30" t="s">
         <v>47</v>
       </c>
-      <c r="P19" s="22"/>
-      <c r="Q19" s="22"/>
-      <c r="R19" s="38"/>
-      <c r="S19" s="37"/>
-      <c r="T19" s="31"/>
-      <c r="U19" s="31"/>
-      <c r="V19" s="31"/>
-      <c r="W19" s="47"/>
-      <c r="X19" s="37"/>
-      <c r="Y19" s="32"/>
-      <c r="Z19" s="32"/>
-      <c r="AA19" s="32"/>
-      <c r="AB19" s="50"/>
+      <c r="P19" s="30"/>
+      <c r="Q19" s="30"/>
+      <c r="R19" s="31"/>
+      <c r="S19" s="21"/>
+      <c r="T19" s="19"/>
+      <c r="U19" s="19"/>
+      <c r="V19" s="19"/>
+      <c r="W19" s="26"/>
+      <c r="X19" s="21"/>
+      <c r="Y19" s="20"/>
+      <c r="Z19" s="20"/>
+      <c r="AA19" s="20"/>
+      <c r="AB19" s="28"/>
     </row>
-    <row r="20" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D20" s="37"/>
+    <row r="20" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D20" s="21"/>
       <c r="E20" s="13"/>
       <c r="F20" s="13"/>
       <c r="G20" s="13"/>
-      <c r="H20" s="39"/>
-      <c r="I20" s="37"/>
+      <c r="H20" s="22"/>
+      <c r="I20" s="21"/>
       <c r="J20" s="13"/>
       <c r="K20" s="13"/>
       <c r="L20" s="13"/>
-      <c r="M20" s="39"/>
-      <c r="N20" s="45"/>
-      <c r="O20" s="22" t="s">
+      <c r="M20" s="22"/>
+      <c r="N20" s="25"/>
+      <c r="O20" s="30" t="s">
         <v>48</v>
       </c>
-      <c r="P20" s="22"/>
-      <c r="Q20" s="22"/>
-      <c r="R20" s="38"/>
-      <c r="S20" s="37"/>
-      <c r="T20" s="31"/>
-      <c r="U20" s="31"/>
-      <c r="V20" s="31"/>
-      <c r="W20" s="47"/>
-      <c r="X20" s="37"/>
-      <c r="Y20" s="32"/>
-      <c r="Z20" s="32"/>
-      <c r="AA20" s="32"/>
-      <c r="AB20" s="50"/>
+      <c r="P20" s="30"/>
+      <c r="Q20" s="30"/>
+      <c r="R20" s="31"/>
+      <c r="S20" s="21"/>
+      <c r="T20" s="19"/>
+      <c r="U20" s="19"/>
+      <c r="V20" s="19"/>
+      <c r="W20" s="26"/>
+      <c r="X20" s="21"/>
+      <c r="Y20" s="20"/>
+      <c r="Z20" s="20"/>
+      <c r="AA20" s="20"/>
+      <c r="AB20" s="28"/>
     </row>
-    <row r="21" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D21" s="37"/>
+    <row r="21" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D21" s="21"/>
       <c r="E21" s="13"/>
       <c r="F21" s="13"/>
       <c r="G21" s="13"/>
-      <c r="H21" s="39"/>
-      <c r="I21" s="37"/>
+      <c r="H21" s="22"/>
+      <c r="I21" s="21"/>
       <c r="J21" s="13"/>
       <c r="K21" s="13"/>
       <c r="L21" s="13"/>
-      <c r="M21" s="39"/>
-      <c r="N21" s="45"/>
-      <c r="O21" s="22" t="s">
+      <c r="M21" s="22"/>
+      <c r="N21" s="25"/>
+      <c r="O21" s="30" t="s">
         <v>49</v>
       </c>
-      <c r="P21" s="22"/>
-      <c r="Q21" s="22"/>
-      <c r="R21" s="38"/>
-      <c r="S21" s="37"/>
-      <c r="T21" s="31"/>
-      <c r="U21" s="31"/>
-      <c r="V21" s="31"/>
-      <c r="W21" s="47"/>
-      <c r="X21" s="37"/>
-      <c r="Y21" s="32"/>
-      <c r="Z21" s="32"/>
-      <c r="AA21" s="32"/>
-      <c r="AB21" s="50"/>
+      <c r="P21" s="30"/>
+      <c r="Q21" s="30"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="21"/>
+      <c r="T21" s="19"/>
+      <c r="U21" s="19"/>
+      <c r="V21" s="19"/>
+      <c r="W21" s="26"/>
+      <c r="X21" s="21"/>
+      <c r="Y21" s="20"/>
+      <c r="Z21" s="20"/>
+      <c r="AA21" s="20"/>
+      <c r="AB21" s="28"/>
     </row>
-    <row r="22" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D22" s="37"/>
+    <row r="22" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D22" s="21"/>
       <c r="E22" s="13"/>
       <c r="F22" s="13"/>
       <c r="G22" s="13"/>
-      <c r="H22" s="39"/>
-      <c r="I22" s="37"/>
+      <c r="H22" s="22"/>
+      <c r="I22" s="21"/>
       <c r="J22" s="13"/>
       <c r="K22" s="13"/>
       <c r="L22" s="13"/>
-      <c r="M22" s="39"/>
-      <c r="N22" s="45"/>
-      <c r="O22" s="22" t="s">
+      <c r="M22" s="22"/>
+      <c r="N22" s="25"/>
+      <c r="O22" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="P22" s="22"/>
-      <c r="Q22" s="22"/>
-      <c r="R22" s="38"/>
-      <c r="S22" s="37"/>
-      <c r="T22" s="31"/>
-      <c r="U22" s="31"/>
-      <c r="V22" s="31"/>
-      <c r="W22" s="47"/>
-      <c r="X22" s="37"/>
-      <c r="Y22" s="32"/>
-      <c r="Z22" s="32"/>
-      <c r="AA22" s="32"/>
-      <c r="AB22" s="50"/>
+      <c r="P22" s="30"/>
+      <c r="Q22" s="30"/>
+      <c r="R22" s="31"/>
+      <c r="S22" s="21"/>
+      <c r="T22" s="19"/>
+      <c r="U22" s="19"/>
+      <c r="V22" s="19"/>
+      <c r="W22" s="26"/>
+      <c r="X22" s="21"/>
+      <c r="Y22" s="20"/>
+      <c r="Z22" s="20"/>
+      <c r="AA22" s="20"/>
+      <c r="AB22" s="28"/>
     </row>
-    <row r="23" spans="1:28" ht="32.25" customHeight="1">
-      <c r="D23" s="37"/>
+    <row r="23" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="D23" s="21"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
       <c r="G23" s="14"/>
-      <c r="H23" s="40"/>
-      <c r="I23" s="37"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="21"/>
       <c r="J23" s="14"/>
       <c r="K23" s="14"/>
       <c r="L23" s="14"/>
-      <c r="M23" s="40"/>
-      <c r="N23" s="45"/>
-      <c r="O23" s="22" t="s">
+      <c r="M23" s="23"/>
+      <c r="N23" s="25"/>
+      <c r="O23" s="30" t="s">
         <v>50</v>
       </c>
-      <c r="P23" s="22"/>
-      <c r="Q23" s="22"/>
-      <c r="R23" s="38"/>
-      <c r="S23" s="37"/>
+      <c r="P23" s="30"/>
+      <c r="Q23" s="30"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="21"/>
       <c r="T23" s="15"/>
       <c r="U23" s="15"/>
       <c r="V23" s="15"/>
-      <c r="W23" s="48"/>
-      <c r="X23" s="37"/>
+      <c r="W23" s="27"/>
+      <c r="X23" s="21"/>
       <c r="Y23" s="16"/>
       <c r="Z23" s="16"/>
       <c r="AA23" s="16"/>
-      <c r="AB23" s="51"/>
+      <c r="AB23" s="29"/>
     </row>
-    <row r="24" spans="1:28" ht="51.75" customHeight="1">
-      <c r="A24" s="23" t="s">
+    <row r="24" spans="1:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A24" s="36" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="23"/>
-      <c r="D24" s="24" t="s">
+      <c r="B24" s="36"/>
+      <c r="D24" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="25"/>
-      <c r="F24" s="25"/>
-      <c r="G24" s="25"/>
-      <c r="H24" s="26"/>
-      <c r="I24" s="24"/>
-      <c r="J24" s="25"/>
-      <c r="K24" s="25"/>
-      <c r="L24" s="25"/>
-      <c r="M24" s="26"/>
-      <c r="N24" s="24" t="s">
+      <c r="E24" s="33"/>
+      <c r="F24" s="33"/>
+      <c r="G24" s="33"/>
+      <c r="H24" s="34"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="33"/>
+      <c r="K24" s="33"/>
+      <c r="L24" s="33"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="O24" s="25"/>
-      <c r="P24" s="25"/>
-      <c r="Q24" s="25"/>
-      <c r="R24" s="26"/>
-      <c r="S24" s="24"/>
-      <c r="T24" s="25"/>
-      <c r="U24" s="25"/>
-      <c r="V24" s="25"/>
-      <c r="W24" s="26"/>
-      <c r="X24" s="24"/>
-      <c r="Y24" s="25"/>
-      <c r="Z24" s="25"/>
-      <c r="AA24" s="25"/>
-      <c r="AB24" s="26"/>
+      <c r="O24" s="33"/>
+      <c r="P24" s="33"/>
+      <c r="Q24" s="33"/>
+      <c r="R24" s="34"/>
+      <c r="S24" s="32"/>
+      <c r="T24" s="33"/>
+      <c r="U24" s="33"/>
+      <c r="V24" s="33"/>
+      <c r="W24" s="34"/>
+      <c r="X24" s="32"/>
+      <c r="Y24" s="33"/>
+      <c r="Z24" s="33"/>
+      <c r="AA24" s="33"/>
+      <c r="AB24" s="34"/>
     </row>
-    <row r="25" spans="1:28" s="7" customFormat="1" ht="11.25" customHeight="1">
+    <row r="25" spans="1:28" s="7" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
       <c r="D25" s="10"/>
       <c r="E25" s="10"/>
@@ -3436,37 +3473,37 @@
       <c r="V25" s="11"/>
       <c r="W25" s="11"/>
     </row>
-    <row r="26" spans="1:28" ht="15" customHeight="1">
+    <row r="26" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M26" s="7"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="22"/>
-      <c r="P26" s="22"/>
-      <c r="Q26" s="22"/>
-      <c r="R26" s="22"/>
+      <c r="O26" s="30"/>
+      <c r="P26" s="30"/>
+      <c r="Q26" s="30"/>
+      <c r="R26" s="30"/>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
       <c r="V26" s="5"/>
       <c r="W26" s="5"/>
     </row>
-    <row r="27" spans="1:28" ht="15" customHeight="1">
+    <row r="27" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M27" s="7"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="22"/>
-      <c r="P27" s="22"/>
-      <c r="Q27" s="22"/>
-      <c r="R27" s="22"/>
+      <c r="O27" s="30"/>
+      <c r="P27" s="30"/>
+      <c r="Q27" s="30"/>
+      <c r="R27" s="30"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
       <c r="V27" s="5"/>
       <c r="W27" s="5"/>
     </row>
-    <row r="28" spans="1:28">
-      <c r="A28" s="17" t="s">
+    <row r="28" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A28" s="35" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="17"/>
+      <c r="B28" s="35"/>
       <c r="C28" s="12"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
@@ -3480,7 +3517,7 @@
       <c r="V28" s="5"/>
       <c r="W28" s="5"/>
     </row>
-    <row r="29" spans="1:28" ht="27" customHeight="1">
+    <row r="29" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D29" s="2"/>
       <c r="E29" s="2" t="s">
         <v>0</v>
@@ -3492,10 +3529,10 @@
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
       <c r="U29" s="5"/>
-      <c r="V29" s="22"/>
-      <c r="W29" s="22"/>
+      <c r="V29" s="30"/>
+      <c r="W29" s="30"/>
     </row>
-    <row r="30" spans="1:28" ht="27" customHeight="1">
+    <row r="30" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="2"/>
       <c r="E30" s="2" t="s">
         <v>6</v>
@@ -3512,7 +3549,7 @@
       <c r="V30" s="5"/>
       <c r="W30" s="5"/>
     </row>
-    <row r="31" spans="1:28" ht="27" customHeight="1">
+    <row r="31" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E31" s="2" t="s">
         <v>5</v>
       </c>
@@ -3527,7 +3564,7 @@
       <c r="V31" s="5"/>
       <c r="W31" s="5"/>
     </row>
-    <row r="32" spans="1:28" ht="27" customHeight="1">
+    <row r="32" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E32" s="2" t="s">
         <v>4</v>
       </c>
@@ -3541,7 +3578,7 @@
       <c r="V32" s="5"/>
       <c r="W32" s="5"/>
     </row>
-    <row r="33" spans="5:23" ht="27" customHeight="1">
+    <row r="33" spans="5:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E33" s="2" t="s">
         <v>1</v>
       </c>
@@ -3556,7 +3593,7 @@
       <c r="V33" s="5"/>
       <c r="W33" s="5"/>
     </row>
-    <row r="34" spans="5:23" ht="27" customHeight="1">
+    <row r="34" spans="5:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E34" s="2" t="s">
         <v>7</v>
       </c>
@@ -3571,7 +3608,7 @@
       <c r="V34" s="5"/>
       <c r="W34" s="5"/>
     </row>
-    <row r="35" spans="5:23" ht="27" customHeight="1">
+    <row r="35" spans="5:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E35" s="2" t="s">
         <v>2</v>
       </c>
@@ -3586,7 +3623,7 @@
       <c r="V35" s="5"/>
       <c r="W35" s="5"/>
     </row>
-    <row r="36" spans="5:23" ht="27" customHeight="1">
+    <row r="36" spans="5:23" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="E36" s="2" t="s">
         <v>3</v>
       </c>
@@ -3601,12 +3638,67 @@
       <c r="V36" s="5"/>
       <c r="W36" s="5"/>
     </row>
-    <row r="37" spans="5:23">
+    <row r="37" spans="5:23" x14ac:dyDescent="0.25">
       <c r="E37" s="2"/>
       <c r="F37" s="2"/>
     </row>
   </sheetData>
-  <mergeCells count="62">
+  <mergeCells count="63">
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="S5:W5"/>
+    <mergeCell ref="X5:AB5"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="S4:W4"/>
+    <mergeCell ref="E15:H15"/>
+    <mergeCell ref="J15:M15"/>
+    <mergeCell ref="T15:W15"/>
+    <mergeCell ref="Y15:AB15"/>
+    <mergeCell ref="T7:W7"/>
+    <mergeCell ref="Y7:AB7"/>
+    <mergeCell ref="J7:M7"/>
+    <mergeCell ref="E7:H7"/>
+    <mergeCell ref="O7:R7"/>
+    <mergeCell ref="T11:W11"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="I24:M24"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="S24:W24"/>
+    <mergeCell ref="Y8:AB8"/>
+    <mergeCell ref="Y10:AB10"/>
+    <mergeCell ref="Y11:AB11"/>
+    <mergeCell ref="O26:R26"/>
+    <mergeCell ref="O27:R27"/>
+    <mergeCell ref="X24:AB24"/>
+    <mergeCell ref="Y9:AB9"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="O13:R13"/>
+    <mergeCell ref="O14:R14"/>
+    <mergeCell ref="O8:R8"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="O15:R15"/>
     <mergeCell ref="O21:R21"/>
     <mergeCell ref="O22:R22"/>
     <mergeCell ref="O23:R23"/>
@@ -3615,60 +3707,6 @@
     <mergeCell ref="O18:R18"/>
     <mergeCell ref="O19:R19"/>
     <mergeCell ref="O20:R20"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="Y8:AB8"/>
-    <mergeCell ref="Y10:AB10"/>
-    <mergeCell ref="Y11:AB11"/>
-    <mergeCell ref="O26:R26"/>
-    <mergeCell ref="O27:R27"/>
-    <mergeCell ref="X24:AB24"/>
-    <mergeCell ref="Y9:AB9"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="T9:W9"/>
-    <mergeCell ref="O13:R13"/>
-    <mergeCell ref="O14:R14"/>
-    <mergeCell ref="O8:R8"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="I24:M24"/>
-    <mergeCell ref="N24:R24"/>
-    <mergeCell ref="S24:W24"/>
-    <mergeCell ref="E15:H15"/>
-    <mergeCell ref="J15:M15"/>
-    <mergeCell ref="T15:W15"/>
-    <mergeCell ref="Y15:AB15"/>
-    <mergeCell ref="T7:W7"/>
-    <mergeCell ref="Y7:AB7"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="S4:W4"/>
-    <mergeCell ref="X4:AB4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="S5:W5"/>
-    <mergeCell ref="X5:AB5"/>
-    <mergeCell ref="J7:M7"/>
-    <mergeCell ref="E7:H7"/>
-    <mergeCell ref="O7:R7"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:AB6">
     <cfRule type="expression" dxfId="1" priority="7">

</xml_diff>

<commit_message>
# Updated MapaEntregables.xlsx # Added Estilo propuesto App
</commit_message>
<xml_diff>
--- a/docs/MapaEntregables.xlsx
+++ b/docs/MapaEntregables.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always" codeName="ThisWorkbook" autoCompressPictures="0" defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Damian\Documents\UBA\2do Cuat 2013\TallerDesarrollo2\docs\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Facu\Materias Actuales\75.47 - Taller de Desarrollo de Proyectos II\Repositorio\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="56">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="60">
   <si>
     <t>Code/Implementation</t>
   </si>
@@ -129,12 +129,6 @@
     <t>30 Sep - 21 Oct</t>
   </si>
   <si>
-    <t>21 Oct - 28 Oct</t>
-  </si>
-  <si>
-    <t>28 Oct - 11 Oct</t>
-  </si>
-  <si>
     <t>Ver lista de películas cargadas (servidor)</t>
   </si>
   <si>
@@ -226,6 +220,24 @@
   </si>
   <si>
     <t>Administración de promociones</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Reporte Ventas/Reservas Por Función </t>
+  </si>
+  <si>
+    <t>Reporte Horarios Más Vendidos</t>
+  </si>
+  <si>
+    <t>Reporte Entradas más vendidas por película</t>
+  </si>
+  <si>
+    <t>4 Nov - 11 Nov</t>
+  </si>
+  <si>
+    <t>21 Oct - 4 Nov</t>
+  </si>
+  <si>
+    <t>Admin. Listar Reportes</t>
   </si>
 </sst>
 </file>
@@ -531,12 +543,48 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -545,42 +593,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="166" fontId="5" fillId="2" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="165" fontId="5" fillId="2" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1361,216 +1373,6 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>87923</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>65943</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>302236</xdr:colOff>
-      <xdr:row>6</xdr:row>
-      <xdr:rowOff>298509</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="43" name="Picture 42" descr="document_text_32.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8264769" y="1208943"/>
-          <a:ext cx="214313" cy="232566"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>87923</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>43962</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>302236</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>276528</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="45" name="Picture 44" descr="document_text_32.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8264769" y="1567962"/>
-          <a:ext cx="214313" cy="232566"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>95250</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>7327</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>309563</xdr:colOff>
-      <xdr:row>8</xdr:row>
-      <xdr:rowOff>239893</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="46" name="Picture 45" descr="document_text_32.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8272096" y="1912327"/>
-          <a:ext cx="214313" cy="232566"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>95249</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>43962</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>309562</xdr:colOff>
-      <xdr:row>9</xdr:row>
-      <xdr:rowOff>276528</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="47" name="Picture 46" descr="document_text_32.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8272095" y="2242039"/>
-          <a:ext cx="214313" cy="232566"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>87923</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>7327</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>23</xdr:col>
-      <xdr:colOff>302236</xdr:colOff>
-      <xdr:row>10</xdr:row>
-      <xdr:rowOff>239893</xdr:rowOff>
-    </xdr:to>
-    <xdr:pic>
-      <xdr:nvPicPr>
-        <xdr:cNvPr id="49" name="Picture 48" descr="document_text_32.png"/>
-        <xdr:cNvPicPr>
-          <a:picLocks noChangeAspect="1"/>
-        </xdr:cNvPicPr>
-      </xdr:nvPicPr>
-      <xdr:blipFill>
-        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print"/>
-        <a:stretch>
-          <a:fillRect/>
-        </a:stretch>
-      </xdr:blipFill>
-      <xdr:spPr>
-        <a:xfrm>
-          <a:off x="8264769" y="2586404"/>
-          <a:ext cx="214313" cy="232566"/>
-        </a:xfrm>
-        <a:prstGeom prst="rect">
-          <a:avLst/>
-        </a:prstGeom>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-      </xdr:spPr>
-    </xdr:pic>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-  <xdr:twoCellAnchor editAs="oneCell">
-    <xdr:from>
       <xdr:col>3</xdr:col>
       <xdr:colOff>14653</xdr:colOff>
       <xdr:row>6</xdr:row>
@@ -2434,6 +2236,158 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="7403522" y="2623704"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>69273</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>60614</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>283585</xdr:colOff>
+      <xdr:row>6</xdr:row>
+      <xdr:rowOff>287623</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="52" name="Picture 51" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9178637" y="1203614"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>69272</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>86591</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>283584</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>313600</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="53" name="Picture 52" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9178636" y="1610591"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>74467</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>39832</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>288779</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>266841</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="54" name="Picture 53" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9183831" y="1944832"/>
+          <a:ext cx="214312" cy="227009"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>69273</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>69274</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>23</xdr:col>
+      <xdr:colOff>283585</xdr:colOff>
+      <xdr:row>9</xdr:row>
+      <xdr:rowOff>296283</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="56" name="Picture 34" descr="source_code_32.png"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId8" cstate="print"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="9178637" y="2268683"/>
           <a:ext cx="214312" cy="227009"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2767,7 +2721,7 @@
   <dimension ref="A4:AB37"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" zoomScale="110" zoomScaleNormal="110" zoomScalePageLayoutView="90" workbookViewId="0">
-      <selection activeCell="S24" sqref="A4:W24"/>
+      <selection activeCell="AI7" sqref="AI7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2784,82 +2738,82 @@
   </cols>
   <sheetData>
     <row r="4" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A4" s="35" t="s">
+      <c r="A4" s="36" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="35"/>
-      <c r="D4" s="41" t="s">
+      <c r="B4" s="36"/>
+      <c r="D4" s="30" t="s">
         <v>14</v>
       </c>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="43"/>
-      <c r="I4" s="41" t="s">
+      <c r="E4" s="31"/>
+      <c r="F4" s="31"/>
+      <c r="G4" s="31"/>
+      <c r="H4" s="32"/>
+      <c r="I4" s="30" t="s">
         <v>15</v>
       </c>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="43"/>
-      <c r="N4" s="41" t="s">
+      <c r="J4" s="31"/>
+      <c r="K4" s="31"/>
+      <c r="L4" s="31"/>
+      <c r="M4" s="32"/>
+      <c r="N4" s="30" t="s">
         <v>16</v>
       </c>
-      <c r="O4" s="42"/>
-      <c r="P4" s="42"/>
-      <c r="Q4" s="42"/>
-      <c r="R4" s="43"/>
-      <c r="S4" s="41" t="s">
+      <c r="O4" s="31"/>
+      <c r="P4" s="31"/>
+      <c r="Q4" s="31"/>
+      <c r="R4" s="32"/>
+      <c r="S4" s="30" t="s">
         <v>17</v>
       </c>
-      <c r="T4" s="42"/>
-      <c r="U4" s="42"/>
-      <c r="V4" s="42"/>
-      <c r="W4" s="43"/>
-      <c r="X4" s="41" t="s">
+      <c r="T4" s="31"/>
+      <c r="U4" s="31"/>
+      <c r="V4" s="31"/>
+      <c r="W4" s="32"/>
+      <c r="X4" s="30" t="s">
         <v>18</v>
       </c>
-      <c r="Y4" s="42"/>
-      <c r="Z4" s="42"/>
-      <c r="AA4" s="42"/>
-      <c r="AB4" s="43"/>
+      <c r="Y4" s="31"/>
+      <c r="Z4" s="31"/>
+      <c r="AA4" s="31"/>
+      <c r="AB4" s="32"/>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="D5" s="44" t="s">
+      <c r="D5" s="33" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="45"/>
-      <c r="F5" s="45"/>
-      <c r="G5" s="45"/>
-      <c r="H5" s="46"/>
-      <c r="I5" s="44" t="s">
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="33" t="s">
         <v>10</v>
       </c>
-      <c r="J5" s="45"/>
-      <c r="K5" s="45"/>
-      <c r="L5" s="45"/>
-      <c r="M5" s="46"/>
-      <c r="N5" s="44" t="s">
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
+      <c r="M5" s="35"/>
+      <c r="N5" s="33" t="s">
         <v>22</v>
       </c>
-      <c r="O5" s="45"/>
-      <c r="P5" s="45"/>
-      <c r="Q5" s="45"/>
-      <c r="R5" s="46"/>
-      <c r="S5" s="44" t="s">
-        <v>23</v>
-      </c>
-      <c r="T5" s="45"/>
-      <c r="U5" s="45"/>
-      <c r="V5" s="45"/>
-      <c r="W5" s="46"/>
-      <c r="X5" s="44" t="s">
-        <v>24</v>
-      </c>
-      <c r="Y5" s="45"/>
-      <c r="Z5" s="45"/>
-      <c r="AA5" s="45"/>
-      <c r="AB5" s="46"/>
+      <c r="O5" s="34"/>
+      <c r="P5" s="34"/>
+      <c r="Q5" s="34"/>
+      <c r="R5" s="35"/>
+      <c r="S5" s="33" t="s">
+        <v>58</v>
+      </c>
+      <c r="T5" s="34"/>
+      <c r="U5" s="34"/>
+      <c r="V5" s="34"/>
+      <c r="W5" s="35"/>
+      <c r="X5" s="33" t="s">
+        <v>57</v>
+      </c>
+      <c r="Y5" s="34"/>
+      <c r="Z5" s="34"/>
+      <c r="AA5" s="34"/>
+      <c r="AB5" s="35"/>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.25">
       <c r="D6" s="4"/>
@@ -2890,108 +2844,114 @@
     </row>
     <row r="7" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D7" s="21"/>
-      <c r="E7" s="30" t="s">
+      <c r="E7" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="F7" s="30"/>
-      <c r="G7" s="30"/>
-      <c r="H7" s="31"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="37"/>
+      <c r="H7" s="38"/>
       <c r="I7" s="21"/>
-      <c r="J7" s="30" t="s">
-        <v>27</v>
-      </c>
-      <c r="K7" s="30"/>
-      <c r="L7" s="30"/>
-      <c r="M7" s="31"/>
+      <c r="J7" s="37" t="s">
+        <v>25</v>
+      </c>
+      <c r="K7" s="37"/>
+      <c r="L7" s="37"/>
+      <c r="M7" s="38"/>
       <c r="N7" s="21"/>
-      <c r="O7" s="30" t="s">
-        <v>35</v>
-      </c>
-      <c r="P7" s="30"/>
-      <c r="Q7" s="30"/>
-      <c r="R7" s="31"/>
+      <c r="O7" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="P7" s="37"/>
+      <c r="Q7" s="37"/>
+      <c r="R7" s="38"/>
       <c r="S7" s="21"/>
-      <c r="T7" s="30" t="s">
-        <v>51</v>
-      </c>
-      <c r="U7" s="30"/>
-      <c r="V7" s="30"/>
-      <c r="W7" s="31"/>
+      <c r="T7" s="37" t="s">
+        <v>49</v>
+      </c>
+      <c r="U7" s="37"/>
+      <c r="V7" s="37"/>
+      <c r="W7" s="38"/>
       <c r="X7" s="21"/>
-      <c r="Y7" s="30"/>
-      <c r="Z7" s="30"/>
-      <c r="AA7" s="30"/>
-      <c r="AB7" s="31"/>
+      <c r="Y7" s="37" t="s">
+        <v>54</v>
+      </c>
+      <c r="Z7" s="37"/>
+      <c r="AA7" s="37"/>
+      <c r="AB7" s="38"/>
     </row>
     <row r="8" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D8" s="21"/>
-      <c r="E8" s="30" t="s">
+      <c r="E8" s="37" t="s">
         <v>12</v>
       </c>
-      <c r="F8" s="30"/>
-      <c r="G8" s="30"/>
-      <c r="H8" s="31"/>
+      <c r="F8" s="37"/>
+      <c r="G8" s="37"/>
+      <c r="H8" s="38"/>
       <c r="I8" s="21"/>
-      <c r="J8" s="30" t="s">
-        <v>25</v>
-      </c>
-      <c r="K8" s="30"/>
-      <c r="L8" s="30"/>
-      <c r="M8" s="31"/>
+      <c r="J8" s="37" t="s">
+        <v>23</v>
+      </c>
+      <c r="K8" s="37"/>
+      <c r="L8" s="37"/>
+      <c r="M8" s="38"/>
       <c r="N8" s="25"/>
-      <c r="O8" s="30" t="s">
-        <v>36</v>
-      </c>
-      <c r="P8" s="30"/>
-      <c r="Q8" s="30"/>
-      <c r="R8" s="31"/>
+      <c r="O8" s="37" t="s">
+        <v>34</v>
+      </c>
+      <c r="P8" s="37"/>
+      <c r="Q8" s="37"/>
+      <c r="R8" s="38"/>
       <c r="S8" s="21"/>
-      <c r="T8" s="30" t="s">
-        <v>52</v>
-      </c>
-      <c r="U8" s="30"/>
-      <c r="V8" s="30"/>
-      <c r="W8" s="31"/>
+      <c r="T8" s="37" t="s">
+        <v>50</v>
+      </c>
+      <c r="U8" s="37"/>
+      <c r="V8" s="37"/>
+      <c r="W8" s="38"/>
       <c r="X8" s="21"/>
-      <c r="Y8" s="30"/>
-      <c r="Z8" s="30"/>
-      <c r="AA8" s="30"/>
-      <c r="AB8" s="31"/>
+      <c r="Y8" s="37" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z8" s="37"/>
+      <c r="AA8" s="37"/>
+      <c r="AB8" s="38"/>
     </row>
     <row r="9" spans="1:28" ht="23.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D9" s="21"/>
-      <c r="E9" s="30" t="s">
+      <c r="E9" s="37" t="s">
         <v>13</v>
       </c>
-      <c r="F9" s="30"/>
-      <c r="G9" s="30"/>
-      <c r="H9" s="31"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="38"/>
       <c r="I9" s="21"/>
-      <c r="J9" s="30" t="s">
-        <v>26</v>
-      </c>
-      <c r="K9" s="30"/>
-      <c r="L9" s="30"/>
-      <c r="M9" s="31"/>
+      <c r="J9" s="37" t="s">
+        <v>24</v>
+      </c>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="38"/>
       <c r="N9" s="25"/>
-      <c r="O9" s="30" t="s">
-        <v>37</v>
-      </c>
-      <c r="P9" s="30"/>
-      <c r="Q9" s="30"/>
-      <c r="R9" s="31"/>
+      <c r="O9" s="37" t="s">
+        <v>35</v>
+      </c>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="38"/>
       <c r="S9" s="21"/>
-      <c r="T9" s="30" t="s">
-        <v>53</v>
-      </c>
-      <c r="U9" s="30"/>
-      <c r="V9" s="30"/>
-      <c r="W9" s="31"/>
+      <c r="T9" s="37" t="s">
+        <v>51</v>
+      </c>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="38"/>
       <c r="X9" s="21"/>
-      <c r="Y9" s="30"/>
-      <c r="Z9" s="30"/>
-      <c r="AA9" s="30"/>
-      <c r="AB9" s="31"/>
+      <c r="Y9" s="37" t="s">
+        <v>56</v>
+      </c>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="38"/>
     </row>
     <row r="10" spans="1:28" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="21"/>
@@ -3000,31 +2960,33 @@
       <c r="G10" s="13"/>
       <c r="H10" s="22"/>
       <c r="I10" s="21"/>
-      <c r="J10" s="30" t="s">
-        <v>28</v>
-      </c>
-      <c r="K10" s="30"/>
-      <c r="L10" s="30"/>
-      <c r="M10" s="31"/>
+      <c r="J10" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="K10" s="37"/>
+      <c r="L10" s="37"/>
+      <c r="M10" s="38"/>
       <c r="N10" s="25"/>
-      <c r="O10" s="30" t="s">
-        <v>38</v>
-      </c>
-      <c r="P10" s="30"/>
-      <c r="Q10" s="30"/>
-      <c r="R10" s="31"/>
+      <c r="O10" s="37" t="s">
+        <v>36</v>
+      </c>
+      <c r="P10" s="37"/>
+      <c r="Q10" s="37"/>
+      <c r="R10" s="38"/>
       <c r="S10" s="21"/>
       <c r="T10" s="47" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="U10" s="47"/>
       <c r="V10" s="47"/>
       <c r="W10" s="48"/>
       <c r="X10" s="21"/>
-      <c r="Y10" s="30"/>
-      <c r="Z10" s="30"/>
-      <c r="AA10" s="30"/>
-      <c r="AB10" s="31"/>
+      <c r="Y10" s="37" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z10" s="37"/>
+      <c r="AA10" s="37"/>
+      <c r="AB10" s="38"/>
     </row>
     <row r="11" spans="1:28" ht="30.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D11" s="21"/>
@@ -3033,31 +2995,31 @@
       <c r="G11" s="13"/>
       <c r="H11" s="22"/>
       <c r="I11" s="21"/>
-      <c r="J11" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="K11" s="30"/>
-      <c r="L11" s="30"/>
-      <c r="M11" s="31"/>
+      <c r="J11" s="37" t="s">
+        <v>27</v>
+      </c>
+      <c r="K11" s="37"/>
+      <c r="L11" s="37"/>
+      <c r="M11" s="38"/>
       <c r="N11" s="25"/>
-      <c r="O11" s="30" t="s">
-        <v>39</v>
-      </c>
-      <c r="P11" s="30"/>
-      <c r="Q11" s="30"/>
-      <c r="R11" s="31"/>
+      <c r="O11" s="37" t="s">
+        <v>37</v>
+      </c>
+      <c r="P11" s="37"/>
+      <c r="Q11" s="37"/>
+      <c r="R11" s="38"/>
       <c r="S11" s="21"/>
-      <c r="T11" s="30" t="s">
-        <v>55</v>
-      </c>
-      <c r="U11" s="30"/>
-      <c r="V11" s="30"/>
-      <c r="W11" s="31"/>
+      <c r="T11" s="37" t="s">
+        <v>53</v>
+      </c>
+      <c r="U11" s="37"/>
+      <c r="V11" s="37"/>
+      <c r="W11" s="38"/>
       <c r="X11" s="21"/>
-      <c r="Y11" s="30"/>
-      <c r="Z11" s="30"/>
-      <c r="AA11" s="30"/>
-      <c r="AB11" s="31"/>
+      <c r="Y11" s="37"/>
+      <c r="Z11" s="37"/>
+      <c r="AA11" s="37"/>
+      <c r="AB11" s="38"/>
     </row>
     <row r="12" spans="1:28" ht="28.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D12" s="21"/>
@@ -3066,19 +3028,19 @@
       <c r="G12" s="13"/>
       <c r="H12" s="22"/>
       <c r="I12" s="21"/>
-      <c r="J12" s="30" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" s="30"/>
-      <c r="L12" s="30"/>
-      <c r="M12" s="31"/>
+      <c r="J12" s="37" t="s">
+        <v>28</v>
+      </c>
+      <c r="K12" s="37"/>
+      <c r="L12" s="37"/>
+      <c r="M12" s="38"/>
       <c r="N12" s="25"/>
-      <c r="O12" s="30" t="s">
-        <v>40</v>
-      </c>
-      <c r="P12" s="30"/>
-      <c r="Q12" s="30"/>
-      <c r="R12" s="31"/>
+      <c r="O12" s="37" t="s">
+        <v>38</v>
+      </c>
+      <c r="P12" s="37"/>
+      <c r="Q12" s="37"/>
+      <c r="R12" s="38"/>
       <c r="S12" s="21"/>
       <c r="T12" s="13"/>
       <c r="U12" s="13"/>
@@ -3097,19 +3059,19 @@
       <c r="G13" s="13"/>
       <c r="H13" s="22"/>
       <c r="I13" s="21"/>
-      <c r="J13" s="30" t="s">
-        <v>31</v>
-      </c>
-      <c r="K13" s="30"/>
-      <c r="L13" s="30"/>
-      <c r="M13" s="31"/>
+      <c r="J13" s="37" t="s">
+        <v>29</v>
+      </c>
+      <c r="K13" s="37"/>
+      <c r="L13" s="37"/>
+      <c r="M13" s="38"/>
       <c r="N13" s="21"/>
-      <c r="O13" s="30" t="s">
-        <v>41</v>
-      </c>
-      <c r="P13" s="30"/>
-      <c r="Q13" s="30"/>
-      <c r="R13" s="31"/>
+      <c r="O13" s="37" t="s">
+        <v>39</v>
+      </c>
+      <c r="P13" s="37"/>
+      <c r="Q13" s="37"/>
+      <c r="R13" s="38"/>
       <c r="S13" s="21"/>
       <c r="T13" s="13"/>
       <c r="U13" s="13"/>
@@ -3128,19 +3090,19 @@
       <c r="G14" s="13"/>
       <c r="H14" s="22"/>
       <c r="I14" s="21"/>
-      <c r="J14" s="30" t="s">
-        <v>32</v>
-      </c>
-      <c r="K14" s="30"/>
-      <c r="L14" s="30"/>
-      <c r="M14" s="31"/>
+      <c r="J14" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="K14" s="37"/>
+      <c r="L14" s="37"/>
+      <c r="M14" s="38"/>
       <c r="N14" s="21"/>
-      <c r="O14" s="30" t="s">
-        <v>42</v>
-      </c>
-      <c r="P14" s="30"/>
-      <c r="Q14" s="30"/>
-      <c r="R14" s="31"/>
+      <c r="O14" s="37" t="s">
+        <v>40</v>
+      </c>
+      <c r="P14" s="37"/>
+      <c r="Q14" s="37"/>
+      <c r="R14" s="38"/>
       <c r="S14" s="21"/>
       <c r="T14" s="13"/>
       <c r="U14" s="13"/>
@@ -3154,34 +3116,34 @@
     </row>
     <row r="15" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D15" s="21"/>
-      <c r="E15" s="30"/>
-      <c r="F15" s="30"/>
-      <c r="G15" s="30"/>
-      <c r="H15" s="31"/>
+      <c r="E15" s="37"/>
+      <c r="F15" s="37"/>
+      <c r="G15" s="37"/>
+      <c r="H15" s="38"/>
       <c r="I15" s="21"/>
-      <c r="J15" s="30" t="s">
-        <v>33</v>
-      </c>
-      <c r="K15" s="30"/>
-      <c r="L15" s="30"/>
-      <c r="M15" s="31"/>
+      <c r="J15" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="K15" s="37"/>
+      <c r="L15" s="37"/>
+      <c r="M15" s="38"/>
       <c r="N15" s="25"/>
-      <c r="O15" s="30" t="s">
-        <v>43</v>
-      </c>
-      <c r="P15" s="30"/>
-      <c r="Q15" s="30"/>
-      <c r="R15" s="31"/>
+      <c r="O15" s="37" t="s">
+        <v>41</v>
+      </c>
+      <c r="P15" s="37"/>
+      <c r="Q15" s="37"/>
+      <c r="R15" s="38"/>
       <c r="S15" s="21"/>
-      <c r="T15" s="37"/>
-      <c r="U15" s="37"/>
-      <c r="V15" s="37"/>
-      <c r="W15" s="38"/>
+      <c r="T15" s="39"/>
+      <c r="U15" s="39"/>
+      <c r="V15" s="39"/>
+      <c r="W15" s="40"/>
       <c r="X15" s="21"/>
-      <c r="Y15" s="39"/>
-      <c r="Z15" s="39"/>
-      <c r="AA15" s="39"/>
-      <c r="AB15" s="40"/>
+      <c r="Y15" s="41"/>
+      <c r="Z15" s="41"/>
+      <c r="AA15" s="41"/>
+      <c r="AB15" s="42"/>
     </row>
     <row r="16" spans="1:28" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D16" s="21"/>
@@ -3195,12 +3157,12 @@
       <c r="L16" s="13"/>
       <c r="M16" s="22"/>
       <c r="N16" s="25"/>
-      <c r="O16" s="30" t="s">
-        <v>44</v>
-      </c>
-      <c r="P16" s="30"/>
-      <c r="Q16" s="30"/>
-      <c r="R16" s="31"/>
+      <c r="O16" s="37" t="s">
+        <v>42</v>
+      </c>
+      <c r="P16" s="37"/>
+      <c r="Q16" s="37"/>
+      <c r="R16" s="38"/>
       <c r="S16" s="21"/>
       <c r="T16" s="19"/>
       <c r="U16" s="19"/>
@@ -3224,12 +3186,12 @@
       <c r="L17" s="13"/>
       <c r="M17" s="22"/>
       <c r="N17" s="25"/>
-      <c r="O17" s="30" t="s">
-        <v>45</v>
-      </c>
-      <c r="P17" s="30"/>
-      <c r="Q17" s="30"/>
-      <c r="R17" s="31"/>
+      <c r="O17" s="37" t="s">
+        <v>43</v>
+      </c>
+      <c r="P17" s="37"/>
+      <c r="Q17" s="37"/>
+      <c r="R17" s="38"/>
       <c r="S17" s="21"/>
       <c r="T17" s="19"/>
       <c r="U17" s="19"/>
@@ -3253,12 +3215,12 @@
       <c r="L18" s="13"/>
       <c r="M18" s="22"/>
       <c r="N18" s="25"/>
-      <c r="O18" s="30" t="s">
-        <v>46</v>
-      </c>
-      <c r="P18" s="30"/>
-      <c r="Q18" s="30"/>
-      <c r="R18" s="31"/>
+      <c r="O18" s="37" t="s">
+        <v>44</v>
+      </c>
+      <c r="P18" s="37"/>
+      <c r="Q18" s="37"/>
+      <c r="R18" s="38"/>
       <c r="S18" s="21"/>
       <c r="T18" s="19"/>
       <c r="U18" s="19"/>
@@ -3282,12 +3244,12 @@
       <c r="L19" s="13"/>
       <c r="M19" s="22"/>
       <c r="N19" s="25"/>
-      <c r="O19" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="P19" s="30"/>
-      <c r="Q19" s="30"/>
-      <c r="R19" s="31"/>
+      <c r="O19" s="37" t="s">
+        <v>45</v>
+      </c>
+      <c r="P19" s="37"/>
+      <c r="Q19" s="37"/>
+      <c r="R19" s="38"/>
       <c r="S19" s="21"/>
       <c r="T19" s="19"/>
       <c r="U19" s="19"/>
@@ -3311,12 +3273,12 @@
       <c r="L20" s="13"/>
       <c r="M20" s="22"/>
       <c r="N20" s="25"/>
-      <c r="O20" s="30" t="s">
-        <v>48</v>
-      </c>
-      <c r="P20" s="30"/>
-      <c r="Q20" s="30"/>
-      <c r="R20" s="31"/>
+      <c r="O20" s="37" t="s">
+        <v>46</v>
+      </c>
+      <c r="P20" s="37"/>
+      <c r="Q20" s="37"/>
+      <c r="R20" s="38"/>
       <c r="S20" s="21"/>
       <c r="T20" s="19"/>
       <c r="U20" s="19"/>
@@ -3340,12 +3302,12 @@
       <c r="L21" s="13"/>
       <c r="M21" s="22"/>
       <c r="N21" s="25"/>
-      <c r="O21" s="30" t="s">
-        <v>49</v>
-      </c>
-      <c r="P21" s="30"/>
-      <c r="Q21" s="30"/>
-      <c r="R21" s="31"/>
+      <c r="O21" s="37" t="s">
+        <v>47</v>
+      </c>
+      <c r="P21" s="37"/>
+      <c r="Q21" s="37"/>
+      <c r="R21" s="38"/>
       <c r="S21" s="21"/>
       <c r="T21" s="19"/>
       <c r="U21" s="19"/>
@@ -3369,12 +3331,12 @@
       <c r="L22" s="13"/>
       <c r="M22" s="22"/>
       <c r="N22" s="25"/>
-      <c r="O22" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="P22" s="30"/>
-      <c r="Q22" s="30"/>
-      <c r="R22" s="31"/>
+      <c r="O22" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="P22" s="37"/>
+      <c r="Q22" s="37"/>
+      <c r="R22" s="38"/>
       <c r="S22" s="21"/>
       <c r="T22" s="19"/>
       <c r="U22" s="19"/>
@@ -3398,12 +3360,12 @@
       <c r="L23" s="14"/>
       <c r="M23" s="23"/>
       <c r="N23" s="25"/>
-      <c r="O23" s="30" t="s">
-        <v>50</v>
-      </c>
-      <c r="P23" s="30"/>
-      <c r="Q23" s="30"/>
-      <c r="R23" s="31"/>
+      <c r="O23" s="37" t="s">
+        <v>48</v>
+      </c>
+      <c r="P23" s="37"/>
+      <c r="Q23" s="37"/>
+      <c r="R23" s="38"/>
       <c r="S23" s="21"/>
       <c r="T23" s="15"/>
       <c r="U23" s="15"/>
@@ -3416,39 +3378,39 @@
       <c r="AB23" s="29"/>
     </row>
     <row r="24" spans="1:28" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="36" t="s">
+      <c r="A24" s="43" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="36"/>
-      <c r="D24" s="32" t="s">
+      <c r="B24" s="43"/>
+      <c r="D24" s="44" t="s">
         <v>21</v>
       </c>
-      <c r="E24" s="33"/>
-      <c r="F24" s="33"/>
-      <c r="G24" s="33"/>
-      <c r="H24" s="34"/>
-      <c r="I24" s="32"/>
-      <c r="J24" s="33"/>
-      <c r="K24" s="33"/>
-      <c r="L24" s="33"/>
-      <c r="M24" s="34"/>
-      <c r="N24" s="32" t="s">
-        <v>34</v>
-      </c>
-      <c r="O24" s="33"/>
-      <c r="P24" s="33"/>
-      <c r="Q24" s="33"/>
-      <c r="R24" s="34"/>
-      <c r="S24" s="32"/>
-      <c r="T24" s="33"/>
-      <c r="U24" s="33"/>
-      <c r="V24" s="33"/>
-      <c r="W24" s="34"/>
-      <c r="X24" s="32"/>
-      <c r="Y24" s="33"/>
-      <c r="Z24" s="33"/>
-      <c r="AA24" s="33"/>
-      <c r="AB24" s="34"/>
+      <c r="E24" s="45"/>
+      <c r="F24" s="45"/>
+      <c r="G24" s="45"/>
+      <c r="H24" s="46"/>
+      <c r="I24" s="44"/>
+      <c r="J24" s="45"/>
+      <c r="K24" s="45"/>
+      <c r="L24" s="45"/>
+      <c r="M24" s="46"/>
+      <c r="N24" s="44" t="s">
+        <v>32</v>
+      </c>
+      <c r="O24" s="45"/>
+      <c r="P24" s="45"/>
+      <c r="Q24" s="45"/>
+      <c r="R24" s="46"/>
+      <c r="S24" s="44"/>
+      <c r="T24" s="45"/>
+      <c r="U24" s="45"/>
+      <c r="V24" s="45"/>
+      <c r="W24" s="46"/>
+      <c r="X24" s="44"/>
+      <c r="Y24" s="45"/>
+      <c r="Z24" s="45"/>
+      <c r="AA24" s="45"/>
+      <c r="AB24" s="46"/>
     </row>
     <row r="25" spans="1:28" s="7" customFormat="1" ht="11.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B25" s="9"/>
@@ -3476,10 +3438,10 @@
     <row r="26" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M26" s="7"/>
       <c r="N26" s="3"/>
-      <c r="O26" s="30"/>
-      <c r="P26" s="30"/>
-      <c r="Q26" s="30"/>
-      <c r="R26" s="30"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
       <c r="S26" s="5"/>
       <c r="T26" s="5"/>
       <c r="U26" s="5"/>
@@ -3489,10 +3451,10 @@
     <row r="27" spans="1:28" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="M27" s="7"/>
       <c r="N27" s="3"/>
-      <c r="O27" s="30"/>
-      <c r="P27" s="30"/>
-      <c r="Q27" s="30"/>
-      <c r="R27" s="30"/>
+      <c r="O27" s="37"/>
+      <c r="P27" s="37"/>
+      <c r="Q27" s="37"/>
+      <c r="R27" s="37"/>
       <c r="S27" s="5"/>
       <c r="T27" s="5"/>
       <c r="U27" s="5"/>
@@ -3500,10 +3462,10 @@
       <c r="W27" s="5"/>
     </row>
     <row r="28" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A28" s="35" t="s">
+      <c r="A28" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="B28" s="35"/>
+      <c r="B28" s="36"/>
       <c r="C28" s="12"/>
       <c r="M28" s="7"/>
       <c r="N28" s="7"/>
@@ -3529,8 +3491,8 @@
       <c r="S29" s="6"/>
       <c r="T29" s="6"/>
       <c r="U29" s="5"/>
-      <c r="V29" s="30"/>
-      <c r="W29" s="30"/>
+      <c r="V29" s="37"/>
+      <c r="W29" s="37"/>
     </row>
     <row r="30" spans="1:28" ht="27" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D30" s="2"/>
@@ -3644,17 +3606,42 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="X4:AB4"/>
-    <mergeCell ref="D5:H5"/>
-    <mergeCell ref="I5:M5"/>
-    <mergeCell ref="N5:R5"/>
-    <mergeCell ref="S5:W5"/>
-    <mergeCell ref="X5:AB5"/>
-    <mergeCell ref="A4:B4"/>
-    <mergeCell ref="D4:H4"/>
-    <mergeCell ref="I4:M4"/>
-    <mergeCell ref="N4:R4"/>
-    <mergeCell ref="S4:W4"/>
+    <mergeCell ref="O21:R21"/>
+    <mergeCell ref="O22:R22"/>
+    <mergeCell ref="O23:R23"/>
+    <mergeCell ref="O16:R16"/>
+    <mergeCell ref="O17:R17"/>
+    <mergeCell ref="O18:R18"/>
+    <mergeCell ref="O19:R19"/>
+    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="O9:R9"/>
+    <mergeCell ref="O10:R10"/>
+    <mergeCell ref="O11:R11"/>
+    <mergeCell ref="O12:R12"/>
+    <mergeCell ref="O15:R15"/>
+    <mergeCell ref="E8:H8"/>
+    <mergeCell ref="J8:M8"/>
+    <mergeCell ref="J14:M14"/>
+    <mergeCell ref="E9:H9"/>
+    <mergeCell ref="J10:M10"/>
+    <mergeCell ref="J9:M9"/>
+    <mergeCell ref="J13:M13"/>
+    <mergeCell ref="J11:M11"/>
+    <mergeCell ref="J12:M12"/>
+    <mergeCell ref="X24:AB24"/>
+    <mergeCell ref="Y9:AB9"/>
+    <mergeCell ref="T10:W10"/>
+    <mergeCell ref="T8:W8"/>
+    <mergeCell ref="T9:W9"/>
+    <mergeCell ref="A28:B28"/>
+    <mergeCell ref="V29:W29"/>
+    <mergeCell ref="A24:B24"/>
+    <mergeCell ref="D24:H24"/>
+    <mergeCell ref="I24:M24"/>
+    <mergeCell ref="N24:R24"/>
+    <mergeCell ref="S24:W24"/>
+    <mergeCell ref="O26:R26"/>
+    <mergeCell ref="O27:R27"/>
     <mergeCell ref="E15:H15"/>
     <mergeCell ref="J15:M15"/>
     <mergeCell ref="T15:W15"/>
@@ -3665,48 +3652,23 @@
     <mergeCell ref="E7:H7"/>
     <mergeCell ref="O7:R7"/>
     <mergeCell ref="T11:W11"/>
-    <mergeCell ref="A28:B28"/>
-    <mergeCell ref="V29:W29"/>
-    <mergeCell ref="A24:B24"/>
-    <mergeCell ref="D24:H24"/>
-    <mergeCell ref="I24:M24"/>
-    <mergeCell ref="N24:R24"/>
-    <mergeCell ref="S24:W24"/>
     <mergeCell ref="Y8:AB8"/>
     <mergeCell ref="Y10:AB10"/>
     <mergeCell ref="Y11:AB11"/>
-    <mergeCell ref="O26:R26"/>
-    <mergeCell ref="O27:R27"/>
-    <mergeCell ref="X24:AB24"/>
-    <mergeCell ref="Y9:AB9"/>
-    <mergeCell ref="T10:W10"/>
-    <mergeCell ref="T8:W8"/>
-    <mergeCell ref="T9:W9"/>
     <mergeCell ref="O13:R13"/>
     <mergeCell ref="O14:R14"/>
     <mergeCell ref="O8:R8"/>
-    <mergeCell ref="E8:H8"/>
-    <mergeCell ref="J8:M8"/>
-    <mergeCell ref="J14:M14"/>
-    <mergeCell ref="E9:H9"/>
-    <mergeCell ref="J10:M10"/>
-    <mergeCell ref="J9:M9"/>
-    <mergeCell ref="J13:M13"/>
-    <mergeCell ref="J11:M11"/>
-    <mergeCell ref="J12:M12"/>
-    <mergeCell ref="O9:R9"/>
-    <mergeCell ref="O10:R10"/>
-    <mergeCell ref="O11:R11"/>
-    <mergeCell ref="O12:R12"/>
-    <mergeCell ref="O15:R15"/>
-    <mergeCell ref="O21:R21"/>
-    <mergeCell ref="O22:R22"/>
-    <mergeCell ref="O23:R23"/>
-    <mergeCell ref="O16:R16"/>
-    <mergeCell ref="O17:R17"/>
-    <mergeCell ref="O18:R18"/>
-    <mergeCell ref="O19:R19"/>
-    <mergeCell ref="O20:R20"/>
+    <mergeCell ref="A4:B4"/>
+    <mergeCell ref="D4:H4"/>
+    <mergeCell ref="I4:M4"/>
+    <mergeCell ref="N4:R4"/>
+    <mergeCell ref="S4:W4"/>
+    <mergeCell ref="X4:AB4"/>
+    <mergeCell ref="D5:H5"/>
+    <mergeCell ref="I5:M5"/>
+    <mergeCell ref="N5:R5"/>
+    <mergeCell ref="S5:W5"/>
+    <mergeCell ref="X5:AB5"/>
   </mergeCells>
   <conditionalFormatting sqref="D6:AB6">
     <cfRule type="expression" dxfId="1" priority="7">

</xml_diff>